<commit_message>
dded updated facebook files
</commit_message>
<xml_diff>
--- a/FB Posts.xlsx
+++ b/FB Posts.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="0" windowWidth="21420" windowHeight="17420" tabRatio="868"/>
+    <workbookView xWindow="-400" yWindow="0" windowWidth="22840" windowHeight="7640" tabRatio="868"/>
   </bookViews>
   <sheets>
     <sheet name="FB Posts" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="x" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FB Posts'!$A$3:$T$156</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FB Posts'!$A$3:$T$155</definedName>
   </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="717">
   <si>
     <t>Link</t>
   </si>
@@ -1144,6 +1144,9 @@
     <t>https://www.facebook.com/ShinyHappyHorses/photos/a.174556059251751.36251.170290249678332/415004478540240/?type=1&amp;theater</t>
   </si>
   <si>
+    <t>Amanda</t>
+  </si>
+  <si>
     <t>Resilience to Bugs</t>
   </si>
   <si>
@@ -2177,9 +2180,6 @@
   </si>
   <si>
     <t xml:space="preserve">4Braiding </t>
-  </si>
-  <si>
-    <t>Fbatman</t>
   </si>
 </sst>
 </file>
@@ -2304,7 +2304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2365,12 +2365,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2398,7 +2392,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2480,18 +2474,6 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -2795,12 +2777,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T174"/>
+  <dimension ref="A1:T173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="660" topLeftCell="A87" activePane="bottomLeft"/>
+      <pane ySplit="660" topLeftCell="A118" activePane="bottomLeft"/>
       <selection activeCell="K1" sqref="K1:K1048576"/>
-      <selection pane="bottomLeft" activeCell="M94" sqref="M94"/>
+      <selection pane="bottomLeft" activeCell="Q118" sqref="Q118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0"/>
@@ -2828,25 +2810,25 @@
   <sheetData>
     <row r="1" spans="1:20" s="10" customFormat="1" ht="18" thickBot="1">
       <c r="A1" s="10" t="s">
+        <v>715</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>713</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>714</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>712</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>713</v>
-      </c>
       <c r="D1" s="10" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>2</v>
@@ -2883,19 +2865,19 @@
         <v>3</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>489</v>
-      </c>
-      <c r="M3" s="5">
-        <v>1</v>
+        <v>490</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="Q3" s="22" t="s">
         <v>491</v>
       </c>
-      <c r="Q3" s="22" t="s">
-        <v>490</v>
-      </c>
       <c r="R3" s="32" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="4" spans="1:20" thickBot="1">
@@ -2911,9 +2893,6 @@
       <c r="K5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="5">
-        <v>2</v>
-      </c>
       <c r="O5" s="3" t="s">
         <v>12</v>
       </c>
@@ -2921,7 +2900,7 @@
         <v>11</v>
       </c>
       <c r="R5" s="32" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="6" spans="1:20" thickBot="1">
@@ -2929,19 +2908,16 @@
         <v>25</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>493</v>
-      </c>
-      <c r="M6" s="5">
-        <v>1</v>
+        <v>494</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="Q6" s="22" t="s">
         <v>20</v>
       </c>
       <c r="R6" s="35" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="S6" s="36"/>
       <c r="T6" s="36"/>
@@ -2961,7 +2937,7 @@
         <v>22</v>
       </c>
       <c r="R8" s="32" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="10" spans="1:20" thickBot="1">
@@ -2974,9 +2950,6 @@
       <c r="K10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M10" s="5">
-        <v>1</v>
-      </c>
       <c r="O10" s="3" t="s">
         <v>27</v>
       </c>
@@ -2984,7 +2957,7 @@
         <v>28</v>
       </c>
       <c r="R10" s="32" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="11" spans="1:20" thickBot="1">
@@ -2992,14 +2965,11 @@
         <v>5</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="5">
-        <v>1</v>
-      </c>
       <c r="O11" s="3" t="s">
         <v>31</v>
       </c>
@@ -3007,7 +2977,7 @@
         <v>29</v>
       </c>
       <c r="R11" s="32" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="12" spans="1:20" thickBot="1">
@@ -3020,9 +2990,6 @@
       <c r="K12" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="M12" s="5">
-        <v>1</v>
-      </c>
       <c r="O12" s="3" t="s">
         <v>32</v>
       </c>
@@ -3030,7 +2997,7 @@
         <v>33</v>
       </c>
       <c r="R12" s="32" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="13" spans="1:20" thickBot="1">
@@ -3041,10 +3008,7 @@
         <v>25</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>689</v>
-      </c>
-      <c r="M13" s="5">
-        <v>1</v>
+        <v>690</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>35</v>
@@ -3053,7 +3017,7 @@
         <v>34</v>
       </c>
       <c r="R13" s="32" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="14" spans="1:20" thickBot="1">
@@ -3067,9 +3031,6 @@
         <v>75</v>
       </c>
       <c r="L14" s="14"/>
-      <c r="M14" s="5">
-        <v>1</v>
-      </c>
       <c r="O14" s="3" t="s">
         <v>38</v>
       </c>
@@ -3077,12 +3038,12 @@
         <v>36</v>
       </c>
       <c r="R14" s="32" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="15" spans="1:20" thickBot="1">
       <c r="J15" s="11" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>76</v>
@@ -3094,7 +3055,7 @@
         <v>40</v>
       </c>
       <c r="R15" s="32" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="16" spans="1:20" thickBot="1">
@@ -3112,12 +3073,12 @@
         <v>16</v>
       </c>
       <c r="R16" s="32" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="17" spans="1:18" thickBot="1">
       <c r="J17" s="11" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="K17" s="12" t="s">
         <v>77</v>
@@ -3129,7 +3090,7 @@
         <v>41</v>
       </c>
       <c r="R17" s="32" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="18" spans="1:18" thickBot="1">
@@ -3137,7 +3098,7 @@
         <v>25</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>45</v>
@@ -3146,12 +3107,12 @@
         <v>43</v>
       </c>
       <c r="R18" s="32" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="19" spans="1:18" thickBot="1">
       <c r="J19" s="11" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="K19" s="12" t="s">
         <v>78</v>
@@ -3166,12 +3127,12 @@
         <v>46</v>
       </c>
       <c r="R19" s="32" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="20" spans="1:18" thickBot="1">
       <c r="J20" s="11" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>48</v>
@@ -3186,7 +3147,7 @@
         <v>47</v>
       </c>
       <c r="R20" s="32" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="21" spans="1:18" thickBot="1">
@@ -3199,9 +3160,6 @@
       <c r="K21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M21" s="5">
-        <v>1</v>
-      </c>
       <c r="O21" s="3" t="s">
         <v>53</v>
       </c>
@@ -3209,12 +3167,12 @@
         <v>51</v>
       </c>
       <c r="R21" s="32" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="22" spans="1:18" thickBot="1">
       <c r="J22" s="29" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>73</v>
@@ -3223,10 +3181,10 @@
         <v>54</v>
       </c>
       <c r="Q22" s="22" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="R22" s="32" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="23" spans="1:18" thickBot="1">
@@ -3234,14 +3192,11 @@
         <v>5</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="K23" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="M23" s="5">
-        <v>1</v>
-      </c>
       <c r="O23" s="3" t="s">
         <v>56</v>
       </c>
@@ -3249,12 +3204,12 @@
         <v>55</v>
       </c>
       <c r="R23" s="32" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="24" spans="1:18" thickBot="1">
       <c r="J24" s="11" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>58</v>
@@ -3263,10 +3218,10 @@
         <v>57</v>
       </c>
       <c r="Q24" s="22" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="R24" s="32" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="25" spans="1:18" thickBot="1">
@@ -3274,22 +3229,19 @@
         <v>5</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="K25" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="M25" s="5">
-        <v>1</v>
-      </c>
       <c r="O25" s="3" t="s">
         <v>59</v>
       </c>
       <c r="Q25" s="22" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="R25" s="32" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="26" spans="1:18" thickBot="1">
@@ -3297,22 +3249,19 @@
         <v>5</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="K26" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="O26" s="19" t="s">
         <v>496</v>
       </c>
-      <c r="M26" s="5">
-        <v>1</v>
-      </c>
-      <c r="O26" s="19" t="s">
-        <v>495</v>
-      </c>
       <c r="Q26" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="R26" s="33" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="27" spans="1:18" thickBot="1">
@@ -3326,24 +3275,21 @@
         <v>61</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="M28" s="5">
-        <v>1</v>
+        <v>546</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="R28" s="32" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="29" spans="1:18" thickBot="1">
       <c r="J29" s="11" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K29" s="12" t="s">
         <v>63</v>
@@ -3352,15 +3298,15 @@
         <v>64</v>
       </c>
       <c r="Q29" s="22" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="R29" s="32" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="30" spans="1:18" thickBot="1">
       <c r="J30" s="11" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>66</v>
@@ -3369,10 +3315,10 @@
         <v>65</v>
       </c>
       <c r="Q30" s="22" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="R30" s="32" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="31" spans="1:18" thickBot="1">
@@ -3380,16 +3326,16 @@
         <v>25</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="O31" s="3" t="s">
         <v>67</v>
       </c>
       <c r="Q31" s="22" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="R31" s="32" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="32" spans="1:18" thickBot="1">
@@ -3402,17 +3348,14 @@
       <c r="K32" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="M32" s="5">
-        <v>1</v>
-      </c>
       <c r="O32" s="3" t="s">
         <v>69</v>
       </c>
       <c r="Q32" s="22" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="R32" s="32" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="33" spans="1:18" thickBot="1">
@@ -3426,27 +3369,27 @@
         <v>71</v>
       </c>
       <c r="Q33" s="22" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="R33" s="32" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="16.25" customHeight="1" thickBot="1">
       <c r="J34" s="11" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K34" s="20" t="s">
+        <v>536</v>
+      </c>
+      <c r="O34" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="O34" s="3" t="s">
-        <v>534</v>
-      </c>
       <c r="Q34" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="R34" s="32" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="16.25" customHeight="1" thickBot="1">
@@ -3463,17 +3406,14 @@
       <c r="K36" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="M36" s="5">
-        <v>1</v>
-      </c>
       <c r="O36" s="3" t="s">
         <v>80</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="R36" s="32" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="37" spans="1:18" thickBot="1">
@@ -3487,7 +3427,7 @@
         <v>81</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="38" spans="1:18" thickBot="1">
@@ -3501,27 +3441,27 @@
         <v>84</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="R38" s="32" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="39" spans="1:18" thickBot="1">
       <c r="J39" s="11" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="O39" s="3" t="s">
         <v>85</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="R39" s="32" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="40" spans="1:18" thickBot="1">
@@ -3534,17 +3474,14 @@
       <c r="K40" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="M40" s="5">
-        <v>1</v>
-      </c>
       <c r="O40" s="3" t="s">
         <v>87</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="R40" s="32" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="41" spans="1:18" thickBot="1">
@@ -3558,10 +3495,10 @@
         <v>89</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="R41" s="32" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="42" spans="1:18" thickBot="1">
@@ -3574,17 +3511,14 @@
       <c r="K42" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="M42" s="5">
-        <v>1</v>
-      </c>
       <c r="O42" s="3" t="s">
         <v>92</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="R42" s="32" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="43" spans="1:18" thickBot="1">
@@ -3601,7 +3535,7 @@
         <v>8</v>
       </c>
       <c r="R43" s="32" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="44" spans="1:18" thickBot="1">
@@ -3615,12 +3549,12 @@
         <v>93</v>
       </c>
       <c r="R44" s="32" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="45" spans="1:18" thickBot="1">
       <c r="J45" s="11" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K45" s="12" t="s">
         <v>96</v>
@@ -3632,7 +3566,7 @@
         <v>95</v>
       </c>
       <c r="R45" s="32" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="46" spans="1:18" thickBot="1">
@@ -3645,9 +3579,6 @@
       <c r="K46" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M46" s="5">
-        <v>1</v>
-      </c>
       <c r="O46" s="3" t="s">
         <v>99</v>
       </c>
@@ -3655,7 +3586,7 @@
         <v>100</v>
       </c>
       <c r="R46" s="32" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="47" spans="1:18" thickBot="1">
@@ -3668,9 +3599,6 @@
       <c r="K47" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="M47" s="5">
-        <v>1</v>
-      </c>
       <c r="O47" s="3" t="s">
         <v>103</v>
       </c>
@@ -3678,7 +3606,7 @@
         <v>101</v>
       </c>
       <c r="R47" s="32" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="48" spans="1:18" thickBot="1">
@@ -3695,12 +3623,12 @@
         <v>106</v>
       </c>
       <c r="R48" s="32" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="49" spans="1:18" thickBot="1">
       <c r="J49" s="11" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K49" s="12" t="s">
         <v>108</v>
@@ -3712,15 +3640,15 @@
         <v>107</v>
       </c>
       <c r="R49" s="32" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="50" spans="1:18" thickBot="1">
       <c r="J50" s="11" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K50" s="27" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="O50" s="3" t="s">
         <v>110</v>
@@ -3729,7 +3657,7 @@
         <v>111</v>
       </c>
       <c r="R50" s="32" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="51" spans="1:18" thickBot="1">
@@ -3738,7 +3666,7 @@
         <v>112</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="52" spans="1:18" thickBot="1">
@@ -3755,7 +3683,7 @@
         <v>113</v>
       </c>
       <c r="R52" s="32" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="53" spans="1:18" thickBot="1">
@@ -3772,7 +3700,7 @@
         <v>116</v>
       </c>
       <c r="R53" s="32" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="54" spans="1:18" thickBot="1">
@@ -3803,7 +3731,7 @@
         <v>121</v>
       </c>
       <c r="R55" s="32" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="56" spans="1:18" thickBot="1">
@@ -3820,7 +3748,7 @@
         <v>124</v>
       </c>
       <c r="R56" s="32" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="57" spans="1:18" thickBot="1">
@@ -3833,9 +3761,6 @@
       <c r="K57" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="M57" s="5">
-        <v>1</v>
-      </c>
       <c r="O57" s="3" t="s">
         <v>129</v>
       </c>
@@ -3843,7 +3768,7 @@
         <v>127</v>
       </c>
       <c r="R57" s="32" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="58" spans="1:18" thickBot="1">
@@ -3860,7 +3785,7 @@
         <v>130</v>
       </c>
       <c r="R58" s="32" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="59" spans="1:18" thickBot="1">
@@ -3873,14 +3798,11 @@
       <c r="K59" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="M59" s="5">
-        <v>1</v>
-      </c>
       <c r="Q59" s="21" t="s">
         <v>133</v>
       </c>
       <c r="R59" s="32" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="60" spans="1:18" thickBot="1">
@@ -3893,14 +3815,11 @@
       <c r="K60" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="M60" s="5">
-        <v>1</v>
-      </c>
       <c r="Q60" s="21" t="s">
         <v>135</v>
       </c>
       <c r="R60" s="32" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="61" spans="1:18" thickBot="1">
@@ -3914,12 +3833,12 @@
         <v>137</v>
       </c>
       <c r="R61" s="32" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="62" spans="1:18" thickBot="1">
       <c r="J62" s="11" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="K62" s="12" t="s">
         <v>147</v>
@@ -3936,7 +3855,7 @@
     </row>
     <row r="63" spans="1:18" thickBot="1">
       <c r="J63" s="11" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="K63" s="12" t="s">
         <v>151</v>
@@ -3948,12 +3867,12 @@
         <v>150</v>
       </c>
       <c r="R63" s="32" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="64" spans="1:18" thickBot="1">
       <c r="J64" s="11" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K64" s="12" t="s">
         <v>157</v>
@@ -3965,7 +3884,7 @@
         <v>155</v>
       </c>
       <c r="R64" s="34" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="65" spans="4:18" thickBot="1">
@@ -3978,9 +3897,6 @@
       <c r="K65" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="M65" s="5">
-        <v>1</v>
-      </c>
       <c r="O65" s="3" t="s">
         <v>159</v>
       </c>
@@ -3988,7 +3904,7 @@
         <v>160</v>
       </c>
       <c r="R65" s="32" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="66" spans="4:18" thickBot="1">
@@ -4005,7 +3921,7 @@
         <v>163</v>
       </c>
       <c r="R66" s="32" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="67" spans="4:18" thickBot="1">
@@ -4018,9 +3934,6 @@
       <c r="K67" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="M67" s="5">
-        <v>1</v>
-      </c>
       <c r="O67" s="3" t="s">
         <v>166</v>
       </c>
@@ -4028,7 +3941,7 @@
         <v>164</v>
       </c>
       <c r="R67" s="32" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="68" spans="4:18" thickBot="1">
@@ -4045,7 +3958,7 @@
         <v>169</v>
       </c>
       <c r="R68" s="32" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="69" spans="4:18" thickBot="1">
@@ -4059,7 +3972,7 @@
         <v>180</v>
       </c>
       <c r="R69" s="32" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="70" spans="4:18" thickBot="1">
@@ -4067,18 +3980,18 @@
         <v>196</v>
       </c>
       <c r="K70" s="20" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="Q70" s="23" t="s">
         <v>195</v>
       </c>
       <c r="R70" s="32" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="71" spans="4:18" thickBot="1">
       <c r="J71" s="11" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="K71" s="12" t="s">
         <v>200</v>
@@ -4090,12 +4003,12 @@
         <v>199</v>
       </c>
       <c r="R71" s="32" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="72" spans="4:18" thickBot="1">
       <c r="J72" s="11" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K72" s="12" t="s">
         <v>203</v>
@@ -4104,12 +4017,12 @@
         <v>202</v>
       </c>
       <c r="R72" s="32" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="73" spans="4:18" thickBot="1">
       <c r="J73" s="11" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K73" s="12" t="s">
         <v>206</v>
@@ -4118,12 +4031,12 @@
         <v>205</v>
       </c>
       <c r="R73" s="32" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="74" spans="4:18" thickBot="1">
       <c r="J74" s="11" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="K74" s="12" t="s">
         <v>208</v>
@@ -4135,7 +4048,7 @@
         <v>207</v>
       </c>
       <c r="R74" s="32" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="75" spans="4:18" thickBot="1">
@@ -4152,7 +4065,7 @@
         <v>214</v>
       </c>
       <c r="R75" s="32" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="76" spans="4:18" thickBot="1">
@@ -4169,7 +4082,7 @@
         <v>215</v>
       </c>
       <c r="R76" s="32" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="77" spans="4:18" thickBot="1">
@@ -4186,7 +4099,7 @@
         <v>219</v>
       </c>
       <c r="R77" s="32" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="78" spans="4:18" thickBot="1">
@@ -4203,12 +4116,12 @@
         <v>220</v>
       </c>
       <c r="R78" s="32" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="79" spans="4:18" thickBot="1">
       <c r="J79" s="11" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="K79" s="12" t="s">
         <v>224</v>
@@ -4220,24 +4133,24 @@
         <v>223</v>
       </c>
       <c r="R79" s="32" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="80" spans="4:18" thickBot="1">
       <c r="J80" s="11" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K80" s="20" t="s">
+        <v>538</v>
+      </c>
+      <c r="O80" s="3" t="s">
         <v>537</v>
-      </c>
-      <c r="O80" s="3" t="s">
-        <v>536</v>
       </c>
       <c r="Q80" s="2" t="s">
         <v>225</v>
       </c>
       <c r="R80" s="32" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="81" spans="1:18" thickBot="1">
@@ -4245,7 +4158,7 @@
         <v>25</v>
       </c>
       <c r="K81" s="12" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="O81" s="3" t="s">
         <v>235</v>
@@ -4254,7 +4167,7 @@
         <v>229</v>
       </c>
       <c r="R81" s="32" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="82" spans="1:18" thickBot="1">
@@ -4271,7 +4184,7 @@
         <v>236</v>
       </c>
       <c r="R82" s="32" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="83" spans="1:18" thickBot="1">
@@ -4288,7 +4201,7 @@
         <v>239</v>
       </c>
       <c r="R83" s="32" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="84" spans="1:18" thickBot="1">
@@ -4305,7 +4218,7 @@
         <v>242</v>
       </c>
       <c r="R84" s="32" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="85" spans="1:18" thickBot="1">
@@ -4322,7 +4235,7 @@
         <v>245</v>
       </c>
       <c r="R85" s="32" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="86" spans="1:18" thickBot="1">
@@ -4335,9 +4248,6 @@
       <c r="K86" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="M86" s="5">
-        <v>1</v>
-      </c>
       <c r="O86" s="3" t="s">
         <v>250</v>
       </c>
@@ -4345,7 +4255,7 @@
         <v>248</v>
       </c>
       <c r="R86" s="32" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="87" spans="1:18" thickBot="1">
@@ -4362,7 +4272,7 @@
         <v>251</v>
       </c>
       <c r="R87" s="32" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="88" spans="1:18" thickBot="1">
@@ -4379,7 +4289,7 @@
         <v>255</v>
       </c>
       <c r="R88" s="32" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="89" spans="1:18" thickBot="1">
@@ -4396,7 +4306,7 @@
         <v>257</v>
       </c>
       <c r="R89" s="32" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="90" spans="1:18" thickBot="1">
@@ -4413,7 +4323,7 @@
         <v>259</v>
       </c>
       <c r="R90" s="32" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="91" spans="1:18" thickBot="1">
@@ -4426,17 +4336,14 @@
       <c r="K91" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="M91" s="5">
-        <v>1</v>
-      </c>
       <c r="N91" s="13" t="s">
         <v>261</v>
       </c>
       <c r="Q91" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="R91" s="32" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="92" spans="1:18" thickBot="1">
@@ -4450,7 +4357,7 @@
         <v>266</v>
       </c>
       <c r="R92" s="32" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="93" spans="1:18" thickBot="1">
@@ -4463,9 +4370,6 @@
       <c r="K93" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="M93" s="5">
-        <v>1</v>
-      </c>
       <c r="O93" s="3" t="s">
         <v>270</v>
       </c>
@@ -4473,7 +4377,7 @@
         <v>269</v>
       </c>
       <c r="R93" s="32" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="94" spans="1:18" thickBot="1">
@@ -4493,7 +4397,7 @@
         <v>273</v>
       </c>
       <c r="R94" s="32" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="95" spans="1:18" thickBot="1">
@@ -4510,7 +4414,7 @@
         <v>276</v>
       </c>
       <c r="R95" s="32" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="96" spans="1:18" thickBot="1">
@@ -4530,7 +4434,7 @@
         <v>278</v>
       </c>
       <c r="R96" s="32" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="97" spans="2:20" thickBot="1">
@@ -4544,7 +4448,7 @@
         <v>281</v>
       </c>
       <c r="R97" s="32" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="98" spans="2:20" thickBot="1">
@@ -4561,7 +4465,7 @@
         <v>284</v>
       </c>
       <c r="R98" s="32" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="99" spans="2:20" thickBot="1">
@@ -4581,7 +4485,7 @@
         <v>291</v>
       </c>
       <c r="R99" s="32" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="100" spans="2:20" thickBot="1">
@@ -4598,7 +4502,7 @@
         <v>292</v>
       </c>
       <c r="R100" s="32" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="101" spans="2:20" thickBot="1">
@@ -4606,7 +4510,7 @@
         <v>5</v>
       </c>
       <c r="J101" s="11" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="K101" s="12" t="s">
         <v>298</v>
@@ -4618,7 +4522,7 @@
         <v>297</v>
       </c>
       <c r="R101" s="32" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="102" spans="2:20" thickBot="1">
@@ -4635,7 +4539,7 @@
         <v>302</v>
       </c>
       <c r="R102" s="32" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="103" spans="2:20" thickBot="1">
@@ -4652,7 +4556,7 @@
         <v>307</v>
       </c>
       <c r="R103" s="32" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="104" spans="2:20" thickBot="1">
@@ -4669,7 +4573,7 @@
         <v>312</v>
       </c>
       <c r="R104" s="32" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="105" spans="2:20" thickBot="1">
@@ -4686,7 +4590,7 @@
         <v>315</v>
       </c>
       <c r="R105" s="32" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="106" spans="2:20" thickBot="1">
@@ -4706,7 +4610,7 @@
         <v>322</v>
       </c>
       <c r="R106" s="32" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="107" spans="2:20" thickBot="1">
@@ -4726,7 +4630,7 @@
         <v>326</v>
       </c>
       <c r="R107" s="32" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="108" spans="2:20" thickBot="1">
@@ -4743,7 +4647,7 @@
         <v>329</v>
       </c>
       <c r="R108" s="32" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="109" spans="2:20" s="45" customFormat="1" thickBot="1">
@@ -4765,14 +4669,14 @@
         <v>332</v>
       </c>
       <c r="R109" s="44" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="S109" s="37"/>
       <c r="T109" s="37"/>
     </row>
     <row r="110" spans="2:20" thickBot="1">
       <c r="J110" s="11" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K110" s="12" t="s">
         <v>336</v>
@@ -4784,7 +4688,7 @@
         <v>335</v>
       </c>
       <c r="R110" s="32" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="111" spans="2:20" thickBot="1">
@@ -4801,7 +4705,7 @@
         <v>338</v>
       </c>
       <c r="R111" s="32" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="112" spans="2:20" thickBot="1">
@@ -4821,10 +4725,10 @@
         <v>343</v>
       </c>
       <c r="R112" s="32" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="113" spans="4:20" thickBot="1">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="113" spans="4:18" thickBot="1">
       <c r="J113" s="11" t="s">
         <v>25</v>
       </c>
@@ -4838,10 +4742,10 @@
         <v>346</v>
       </c>
       <c r="R113" s="32" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="114" spans="4:20" thickBot="1">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="114" spans="4:18" thickBot="1">
       <c r="J114" s="11" t="s">
         <v>25</v>
       </c>
@@ -4855,10 +4759,10 @@
         <v>349</v>
       </c>
       <c r="R114" s="32" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="115" spans="4:20" thickBot="1">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="115" spans="4:18" thickBot="1">
       <c r="J115" s="11" t="s">
         <v>18</v>
       </c>
@@ -4872,10 +4776,10 @@
         <v>352</v>
       </c>
       <c r="R115" s="32" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="116" spans="4:20" thickBot="1">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="116" spans="4:18" thickBot="1">
       <c r="D116" s="14" t="s">
         <v>5</v>
       </c>
@@ -4892,10 +4796,10 @@
         <v>355</v>
       </c>
       <c r="R116" s="32" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="117" spans="4:20" thickBot="1">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="117" spans="4:18" thickBot="1">
       <c r="J117" s="11" t="s">
         <v>359</v>
       </c>
@@ -4909,10 +4813,10 @@
         <v>358</v>
       </c>
       <c r="R117" s="32" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="118" spans="4:20" thickBot="1">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="118" spans="4:18" thickBot="1">
       <c r="J118" s="11" t="s">
         <v>25</v>
       </c>
@@ -4926,12 +4830,12 @@
         <v>362</v>
       </c>
       <c r="R118" s="32" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="119" spans="4:20" thickBot="1">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="119" spans="4:18" thickBot="1">
       <c r="J119" s="11" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="K119" s="12" t="s">
         <v>365</v>
@@ -4943,15 +4847,15 @@
         <v>367</v>
       </c>
       <c r="R119" s="32" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="120" spans="4:20" thickBot="1">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="120" spans="4:18" thickBot="1">
       <c r="J120" s="11" t="s">
         <v>25</v>
       </c>
       <c r="K120" s="12" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="O120" s="3" t="s">
         <v>369</v>
@@ -4960,126 +4864,115 @@
         <v>368</v>
       </c>
       <c r="R120" s="32" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="121" spans="4:20" s="49" customFormat="1" thickBot="1">
-      <c r="J121" s="50"/>
-      <c r="K121" s="50"/>
-      <c r="L121" s="51"/>
-      <c r="M121" s="52"/>
-      <c r="N121" s="50"/>
-      <c r="O121" s="52"/>
-      <c r="P121" s="50"/>
-      <c r="Q121" s="53"/>
-      <c r="R121" s="54"/>
-      <c r="S121" s="50"/>
-      <c r="T121" s="50"/>
-    </row>
-    <row r="122" spans="4:20" thickBot="1">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="121" spans="4:18" thickBot="1">
+      <c r="J121" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="K121" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="O121" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q121" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="R121" s="32" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="122" spans="4:18" thickBot="1">
+      <c r="D122" s="14" t="s">
+        <v>5</v>
+      </c>
       <c r="J122" s="11" t="s">
-        <v>609</v>
+        <v>3</v>
       </c>
       <c r="K122" s="12" t="s">
-        <v>372</v>
-      </c>
-      <c r="M122" s="5">
-        <v>2</v>
+        <v>375</v>
       </c>
       <c r="O122" s="3" t="s">
-        <v>716</v>
+        <v>376</v>
       </c>
       <c r="Q122" s="21" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="R122" s="32" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="123" spans="4:20" thickBot="1">
-      <c r="D123" s="14" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="123" spans="4:18" thickBot="1">
+      <c r="J123" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K123" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="Q123" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="R123" s="32" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="124" spans="4:18" thickBot="1">
+      <c r="D124" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J123" s="11" t="s">
+      <c r="J124" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K123" s="12" t="s">
-        <v>374</v>
-      </c>
-      <c r="M123" s="5">
-        <v>2</v>
-      </c>
-      <c r="O123" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q123" s="21" t="s">
-        <v>373</v>
-      </c>
-      <c r="R123" s="32" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="124" spans="4:20" thickBot="1">
-      <c r="J124" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="K124" s="12" t="s">
-        <v>492</v>
-      </c>
-      <c r="M124" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q124" s="21" t="s">
-        <v>376</v>
+        <v>379</v>
+      </c>
+      <c r="Q124" s="22" t="s">
+        <v>378</v>
       </c>
       <c r="R124" s="32" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="125" spans="4:20" thickBot="1">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="125" spans="4:18" thickBot="1">
       <c r="D125" s="14" t="s">
         <v>5</v>
       </c>
       <c r="J125" s="11" t="s">
-        <v>3</v>
+        <v>324</v>
       </c>
       <c r="K125" s="12" t="s">
-        <v>378</v>
-      </c>
-      <c r="M125" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q125" s="22" t="s">
-        <v>377</v>
+        <v>389</v>
+      </c>
+      <c r="O125" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q125" s="21" t="s">
+        <v>387</v>
       </c>
       <c r="R125" s="32" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="126" spans="4:20" thickBot="1">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="126" spans="4:18" thickBot="1">
       <c r="D126" s="14" t="s">
         <v>5</v>
       </c>
       <c r="J126" s="11" t="s">
-        <v>324</v>
+        <v>3</v>
       </c>
       <c r="K126" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="M126" s="5">
-        <v>2</v>
-      </c>
-      <c r="O126" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q126" s="21" t="s">
-        <v>386</v>
+        <v>396</v>
+      </c>
+      <c r="Q126" s="2" t="s">
+        <v>395</v>
       </c>
       <c r="R126" s="32" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="127" spans="4:20" thickBot="1">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="127" spans="4:18" thickBot="1">
       <c r="D127" s="14" t="s">
         <v>5</v>
       </c>
@@ -5087,19 +4980,16 @@
         <v>3</v>
       </c>
       <c r="K127" s="12" t="s">
-        <v>395</v>
-      </c>
-      <c r="M127" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q127" s="2" t="s">
-        <v>394</v>
+        <v>398</v>
+      </c>
+      <c r="Q127" s="21" t="s">
+        <v>397</v>
       </c>
       <c r="R127" s="32" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="128" spans="4:20" thickBot="1">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="128" spans="4:18" thickBot="1">
       <c r="D128" s="14" t="s">
         <v>5</v>
       </c>
@@ -5107,73 +4997,58 @@
         <v>3</v>
       </c>
       <c r="K128" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="M128" s="5">
-        <v>2</v>
-      </c>
-      <c r="Q128" s="21" t="s">
-        <v>396</v>
+        <v>400</v>
+      </c>
+      <c r="Q128" s="22" t="s">
+        <v>399</v>
       </c>
       <c r="R128" s="32" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="129" spans="1:18" thickBot="1">
-      <c r="D129" s="14" t="s">
-        <v>5</v>
-      </c>
       <c r="J129" s="11" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="K129" s="12" t="s">
-        <v>399</v>
-      </c>
-      <c r="M129" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q129" s="22" t="s">
-        <v>398</v>
+        <v>402</v>
+      </c>
+      <c r="Q129" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="R129" s="32" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="130" spans="1:18" thickBot="1">
       <c r="J130" s="11" t="s">
-        <v>18</v>
+        <v>683</v>
       </c>
       <c r="K130" s="12" t="s">
-        <v>401</v>
-      </c>
-      <c r="M130" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q130" s="21" t="s">
-        <v>400</v>
+        <v>411</v>
+      </c>
+      <c r="O130" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q130" s="2" t="s">
+        <v>409</v>
       </c>
       <c r="R130" s="32" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
     <row r="131" spans="1:18" thickBot="1">
       <c r="J131" s="11" t="s">
-        <v>682</v>
+        <v>62</v>
       </c>
       <c r="K131" s="12" t="s">
-        <v>410</v>
-      </c>
-      <c r="M131" s="5">
-        <v>2</v>
-      </c>
-      <c r="O131" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="Q131" s="2" t="s">
-        <v>408</v>
+        <v>413</v>
+      </c>
+      <c r="Q131" s="21" t="s">
+        <v>412</v>
       </c>
       <c r="R131" s="32" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="132" spans="1:18" thickBot="1">
@@ -5181,130 +5056,109 @@
         <v>62</v>
       </c>
       <c r="K132" s="12" t="s">
-        <v>412</v>
-      </c>
-      <c r="M132" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q132" s="21" t="s">
-        <v>411</v>
+        <v>415</v>
+      </c>
+      <c r="Q132" s="22" t="s">
+        <v>414</v>
       </c>
       <c r="R132" s="32" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
     </row>
     <row r="133" spans="1:18" thickBot="1">
       <c r="J133" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="K133" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="O133" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="Q133" s="21" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" thickBot="1">
+      <c r="D134" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J134" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K134" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q134" s="23" t="s">
+        <v>422</v>
+      </c>
+      <c r="R134" s="32" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" thickBot="1">
+      <c r="J135" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K133" s="12" t="s">
-        <v>414</v>
-      </c>
-      <c r="M133" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q133" s="22" t="s">
-        <v>413</v>
-      </c>
-      <c r="R133" s="32" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" thickBot="1">
-      <c r="J134" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="K134" s="12" t="s">
-        <v>418</v>
-      </c>
-      <c r="M134" s="5">
-        <v>2</v>
-      </c>
-      <c r="O134" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q134" s="21" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18" thickBot="1">
-      <c r="D135" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J135" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K135" s="18" t="s">
-        <v>422</v>
-      </c>
-      <c r="M135" s="5">
-        <v>2</v>
-      </c>
-      <c r="Q135" s="23" t="s">
-        <v>421</v>
+      <c r="K135" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="O135" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q135" s="21" t="s">
+        <v>424</v>
       </c>
       <c r="R135" s="32" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="136" spans="1:18" thickBot="1">
       <c r="J136" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K136" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="M136" s="5">
-        <v>1</v>
+        <v>427</v>
       </c>
       <c r="O136" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="Q136" s="21" t="s">
-        <v>423</v>
+        <v>428</v>
+      </c>
+      <c r="Q136" s="22" t="s">
+        <v>429</v>
       </c>
       <c r="R136" s="32" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="137" spans="1:18" thickBot="1">
       <c r="J137" s="11" t="s">
-        <v>61</v>
+        <v>480</v>
       </c>
       <c r="K137" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="M137" s="5">
-        <v>2</v>
+        <v>433</v>
       </c>
       <c r="O137" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="Q137" s="22" t="s">
-        <v>428</v>
+        <v>435</v>
+      </c>
+      <c r="Q137" s="21" t="s">
+        <v>434</v>
       </c>
       <c r="R137" s="32" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
     </row>
     <row r="138" spans="1:18" thickBot="1">
       <c r="J138" s="11" t="s">
-        <v>479</v>
+        <v>25</v>
       </c>
       <c r="K138" s="12" t="s">
-        <v>432</v>
-      </c>
-      <c r="M138" s="5">
-        <v>1</v>
-      </c>
-      <c r="O138" s="3" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="Q138" s="21" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="R138" s="32" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="139" spans="1:18" thickBot="1">
@@ -5312,119 +5166,104 @@
         <v>25</v>
       </c>
       <c r="K139" s="12" t="s">
-        <v>438</v>
-      </c>
-      <c r="M139" s="5">
-        <v>1</v>
+        <v>441</v>
+      </c>
+      <c r="O139" s="3" t="s">
+        <v>442</v>
       </c>
       <c r="Q139" s="21" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="R139" s="32" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="140" spans="1:18" thickBot="1">
       <c r="J140" s="11" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="K140" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="M140" s="5">
-        <v>1</v>
+        <v>444</v>
       </c>
       <c r="O140" s="3" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="Q140" s="21" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="R140" s="32" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="141" spans="1:18" thickBot="1">
       <c r="J141" s="11" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="K141" s="12" t="s">
-        <v>443</v>
-      </c>
-      <c r="M141" s="5">
-        <v>1</v>
-      </c>
-      <c r="O141" s="3" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="Q141" s="21" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="R141" s="32" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="142" spans="1:18" thickBot="1">
+      <c r="D142" s="14" t="s">
+        <v>5</v>
+      </c>
       <c r="J142" s="11" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="K142" s="12" t="s">
-        <v>446</v>
-      </c>
-      <c r="M142" s="5">
-        <v>2</v>
-      </c>
-      <c r="Q142" s="21" t="s">
-        <v>445</v>
+        <v>449</v>
+      </c>
+      <c r="O142" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="Q142" s="2" t="s">
+        <v>527</v>
       </c>
       <c r="R142" s="32" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="143" spans="1:18" thickBot="1">
-      <c r="D143" s="14" t="s">
+      <c r="A143" s="14" t="s">
         <v>5</v>
       </c>
       <c r="J143" s="11" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="K143" s="12" t="s">
-        <v>448</v>
-      </c>
-      <c r="M143" s="5">
-        <v>1</v>
+        <v>451</v>
       </c>
       <c r="O143" s="3" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="Q143" s="2" t="s">
-        <v>526</v>
+        <v>450</v>
       </c>
       <c r="R143" s="32" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="144" spans="1:18" thickBot="1">
-      <c r="A144" s="14" t="s">
+      <c r="D144" s="14" t="s">
         <v>5</v>
       </c>
       <c r="J144" s="11" t="s">
-        <v>61</v>
+        <v>324</v>
       </c>
       <c r="K144" s="12" t="s">
-        <v>450</v>
-      </c>
-      <c r="M144" s="5">
-        <v>1</v>
-      </c>
-      <c r="O144" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="Q144" s="2" t="s">
-        <v>449</v>
+        <v>459</v>
+      </c>
+      <c r="Q144" s="21" t="s">
+        <v>458</v>
       </c>
       <c r="R144" s="32" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="145" spans="2:18" thickBot="1">
@@ -5435,299 +5274,260 @@
         <v>324</v>
       </c>
       <c r="K145" s="12" t="s">
-        <v>458</v>
-      </c>
-      <c r="M145" s="5">
-        <v>1</v>
+        <v>460</v>
+      </c>
+      <c r="O145" s="3" t="s">
+        <v>467</v>
       </c>
       <c r="Q145" s="21" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="R145" s="32" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
     </row>
     <row r="146" spans="2:18" thickBot="1">
-      <c r="D146" s="14" t="s">
-        <v>5</v>
-      </c>
       <c r="J146" s="11" t="s">
-        <v>324</v>
+        <v>25</v>
       </c>
       <c r="K146" s="12" t="s">
-        <v>459</v>
-      </c>
-      <c r="M146" s="5">
-        <v>1</v>
+        <v>462</v>
       </c>
       <c r="O146" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="Q146" s="21" t="s">
-        <v>460</v>
+      <c r="Q146" s="22" t="s">
+        <v>463</v>
       </c>
       <c r="R146" s="32" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="147" spans="2:18" thickBot="1">
+      <c r="D147" s="14" t="s">
+        <v>5</v>
+      </c>
       <c r="J147" s="11" t="s">
         <v>25</v>
       </c>
       <c r="K147" s="12" t="s">
-        <v>461</v>
-      </c>
-      <c r="M147" s="5">
-        <v>1</v>
-      </c>
-      <c r="O147" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="Q147" s="22" t="s">
-        <v>462</v>
+      <c r="Q147" s="2" t="s">
+        <v>464</v>
       </c>
       <c r="R147" s="32" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="148" spans="2:18" thickBot="1">
-      <c r="D148" s="14" t="s">
-        <v>5</v>
-      </c>
       <c r="J148" s="11" t="s">
         <v>25</v>
       </c>
       <c r="K148" s="12" t="s">
-        <v>464</v>
-      </c>
-      <c r="M148" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q148" s="2" t="s">
-        <v>463</v>
+        <v>469</v>
+      </c>
+      <c r="Q148" s="22" t="s">
+        <v>468</v>
       </c>
       <c r="R148" s="32" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="149" spans="2:18" thickBot="1">
       <c r="J149" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K149" s="12" t="s">
-        <v>468</v>
-      </c>
-      <c r="M149" s="5">
-        <v>1</v>
+        <v>472</v>
+      </c>
+      <c r="K149" s="18" t="s">
+        <v>471</v>
+      </c>
+      <c r="O149" s="3" t="s">
+        <v>473</v>
       </c>
       <c r="Q149" s="22" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="R149" s="32" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="150" spans="2:18" thickBot="1">
+      <c r="D150" s="14" t="s">
+        <v>5</v>
+      </c>
       <c r="J150" s="11" t="s">
-        <v>471</v>
+        <v>324</v>
       </c>
       <c r="K150" s="18" t="s">
-        <v>470</v>
-      </c>
-      <c r="M150" s="5">
-        <v>1</v>
+        <v>478</v>
       </c>
       <c r="O150" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="Q150" s="22" t="s">
-        <v>469</v>
+        <v>477</v>
+      </c>
+      <c r="Q150" s="21" t="s">
+        <v>476</v>
       </c>
       <c r="R150" s="32" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="151" spans="2:18" thickBot="1">
-      <c r="D151" s="14" t="s">
-        <v>5</v>
-      </c>
       <c r="J151" s="11" t="s">
-        <v>324</v>
+        <v>480</v>
       </c>
       <c r="K151" s="18" t="s">
-        <v>477</v>
-      </c>
-      <c r="M151" s="5">
-        <v>2</v>
+        <v>481</v>
       </c>
       <c r="O151" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="Q151" s="21" t="s">
-        <v>475</v>
+        <v>678</v>
+      </c>
+      <c r="Q151" s="2" t="s">
+        <v>479</v>
       </c>
       <c r="R151" s="32" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="152" spans="2:18" thickBot="1">
       <c r="J152" s="11" t="s">
-        <v>479</v>
+        <v>62</v>
       </c>
       <c r="K152" s="18" t="s">
-        <v>480</v>
-      </c>
-      <c r="M152" s="5">
-        <v>2</v>
+        <v>483</v>
       </c>
       <c r="O152" s="3" t="s">
-        <v>677</v>
+        <v>484</v>
       </c>
       <c r="Q152" s="2" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="R152" s="32" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
     </row>
     <row r="153" spans="2:18" thickBot="1">
       <c r="J153" s="11" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="K153" s="18" t="s">
-        <v>482</v>
-      </c>
-      <c r="M153" s="5">
-        <v>1</v>
+        <v>486</v>
       </c>
       <c r="O153" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="Q153" s="2" t="s">
-        <v>481</v>
+        <v>487</v>
+      </c>
+      <c r="Q153" s="22" t="s">
+        <v>485</v>
       </c>
       <c r="R153" s="32" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="154" spans="2:18" thickBot="1">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="154" spans="2:18" ht="14">
       <c r="J154" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K154" s="18" t="s">
-        <v>485</v>
-      </c>
-      <c r="M154" s="5">
-        <v>1</v>
-      </c>
-      <c r="O154" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q154" s="22" t="s">
-        <v>484</v>
-      </c>
-      <c r="R154" s="32" t="s">
-        <v>679</v>
+        <v>692</v>
       </c>
     </row>
     <row r="155" spans="2:18" ht="14">
-      <c r="J155" s="11" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="156" spans="2:18" ht="14">
+      <c r="K155" s="12" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="156" spans="2:18" thickBot="1">
       <c r="K156" s="12" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="157" spans="2:18" thickBot="1">
+      <c r="C157" s="14" t="s">
+        <v>5</v>
+      </c>
       <c r="K157" s="12" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="158" spans="2:18" thickBot="1">
-      <c r="C158" s="14" t="s">
+      <c r="B158" s="14" t="s">
         <v>5</v>
       </c>
       <c r="K158" s="12" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="159" spans="2:18" thickBot="1">
-      <c r="B159" s="14" t="s">
+      <c r="C159" s="14" t="s">
         <v>5</v>
       </c>
       <c r="K159" s="12" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
     </row>
     <row r="160" spans="2:18" thickBot="1">
-      <c r="C160" s="14" t="s">
+      <c r="B160" s="14" t="s">
         <v>5</v>
       </c>
       <c r="K160" s="12" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="161" spans="1:18" thickBot="1">
-      <c r="B161" s="14" t="s">
+      <c r="A161" s="14" t="s">
         <v>5</v>
       </c>
       <c r="K161" s="12" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
     </row>
     <row r="162" spans="1:18" thickBot="1">
-      <c r="A162" s="14" t="s">
+      <c r="K162" s="12" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18" thickBot="1">
+      <c r="B163" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K162" s="12" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="163" spans="1:18" thickBot="1">
       <c r="K163" s="12" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="164" spans="1:18" thickBot="1">
-      <c r="B164" s="14" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18" thickBot="1">
+      <c r="C165" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K164" s="12" t="s">
-        <v>700</v>
+      <c r="K165" s="12" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="166" spans="1:18" thickBot="1">
-      <c r="C166" s="14" t="s">
+      <c r="B166" s="14" t="s">
         <v>5</v>
       </c>
       <c r="K166" s="12" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
     </row>
     <row r="167" spans="1:18" thickBot="1">
-      <c r="B167" s="14" t="s">
+      <c r="D167" s="14" t="s">
         <v>5</v>
       </c>
       <c r="K167" s="12" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="168" spans="1:18" thickBot="1">
-      <c r="D168" s="14" t="s">
+      <c r="A168" s="14" t="s">
         <v>5</v>
       </c>
       <c r="K168" s="12" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="169" spans="1:18" thickBot="1">
-      <c r="A169" s="14" t="s">
+      <c r="D169" s="14" t="s">
         <v>5</v>
       </c>
       <c r="K169" s="12" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
     </row>
     <row r="170" spans="1:18" thickBot="1">
@@ -5735,7 +5535,7 @@
         <v>5</v>
       </c>
       <c r="K170" s="12" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
     </row>
     <row r="171" spans="1:18" thickBot="1">
@@ -5743,7 +5543,7 @@
         <v>5</v>
       </c>
       <c r="K171" s="12" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
     </row>
     <row r="172" spans="1:18" thickBot="1">
@@ -5751,26 +5551,18 @@
         <v>5</v>
       </c>
       <c r="K172" s="12" t="s">
-        <v>707</v>
+        <v>709</v>
+      </c>
+      <c r="R172" s="16" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="173" spans="1:18" thickBot="1">
-      <c r="D173" s="14" t="s">
-        <v>5</v>
+      <c r="J173" s="11" t="s">
+        <v>711</v>
       </c>
       <c r="K173" s="12" t="s">
-        <v>708</v>
-      </c>
-      <c r="R173" s="16" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="174" spans="1:18" thickBot="1">
-      <c r="J174" s="11" t="s">
         <v>710</v>
-      </c>
-      <c r="K174" s="12" t="s">
-        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -5786,11 +5578,11 @@
     <hyperlink ref="Q93" r:id="rId9"/>
     <hyperlink ref="Q102" r:id="rId10"/>
     <hyperlink ref="Q113" r:id="rId11"/>
-    <hyperlink ref="Q125" r:id="rId12"/>
-    <hyperlink ref="Q129" r:id="rId13"/>
-    <hyperlink ref="Q133" r:id="rId14"/>
-    <hyperlink ref="Q147" r:id="rId15"/>
-    <hyperlink ref="Q154" r:id="rId16"/>
+    <hyperlink ref="Q124" r:id="rId12"/>
+    <hyperlink ref="Q128" r:id="rId13"/>
+    <hyperlink ref="Q132" r:id="rId14"/>
+    <hyperlink ref="Q146" r:id="rId15"/>
+    <hyperlink ref="Q153" r:id="rId16"/>
     <hyperlink ref="Q26" r:id="rId17"/>
     <hyperlink ref="Q10" r:id="rId18"/>
     <hyperlink ref="Q8" r:id="rId19"/>
@@ -5810,9 +5602,9 @@
     <hyperlink ref="Q32" r:id="rId33"/>
     <hyperlink ref="Q33" r:id="rId34"/>
     <hyperlink ref="Q34" r:id="rId35"/>
-    <hyperlink ref="Q150" r:id="rId36"/>
-    <hyperlink ref="Q149" r:id="rId37"/>
-    <hyperlink ref="Q137" r:id="rId38"/>
+    <hyperlink ref="Q149" r:id="rId36"/>
+    <hyperlink ref="Q148" r:id="rId37"/>
+    <hyperlink ref="Q136" r:id="rId38"/>
     <hyperlink ref="Q50" r:id="rId39"/>
     <hyperlink ref="Q36" r:id="rId40"/>
     <hyperlink ref="Q37" r:id="rId41"/>
@@ -5822,22 +5614,22 @@
     <hyperlink ref="Q41" r:id="rId45"/>
     <hyperlink ref="Q42" r:id="rId46"/>
     <hyperlink ref="Q91" r:id="rId47"/>
-    <hyperlink ref="Q143" r:id="rId48"/>
-    <hyperlink ref="Q144" r:id="rId49"/>
+    <hyperlink ref="Q142" r:id="rId48"/>
+    <hyperlink ref="Q143" r:id="rId49"/>
     <hyperlink ref="Q48" r:id="rId50"/>
     <hyperlink ref="Q51" r:id="rId51"/>
     <hyperlink ref="Q77" r:id="rId52"/>
-    <hyperlink ref="Q127" r:id="rId53"/>
+    <hyperlink ref="Q126" r:id="rId53"/>
     <hyperlink ref="Q90" r:id="rId54"/>
     <hyperlink ref="Q109" r:id="rId55"/>
-    <hyperlink ref="Q153" r:id="rId56"/>
-    <hyperlink ref="Q152" r:id="rId57"/>
-    <hyperlink ref="Q131" r:id="rId58"/>
-    <hyperlink ref="Q148" r:id="rId59"/>
-    <hyperlink ref="R173" r:id="rId60" display="https://www.facebook.com/johanna.jonesfaricelli"/>
+    <hyperlink ref="Q152" r:id="rId56"/>
+    <hyperlink ref="Q151" r:id="rId57"/>
+    <hyperlink ref="Q130" r:id="rId58"/>
+    <hyperlink ref="Q147" r:id="rId59"/>
+    <hyperlink ref="R172" r:id="rId60" display="https://www.facebook.com/johanna.jonesfaricelli"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5881,7 +5673,7 @@
         <v>142</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5916,103 +5708,103 @@
         <v>225</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>381</v>
+      </c>
+      <c r="C10" t="s">
         <v>380</v>
       </c>
-      <c r="C10" t="s">
-        <v>379</v>
-      </c>
       <c r="D10" s="17" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C12" t="s">
         <v>382</v>
       </c>
-      <c r="C12" t="s">
-        <v>381</v>
-      </c>
       <c r="D12" s="17" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C14" t="s">
         <v>391</v>
       </c>
-      <c r="C14" t="s">
-        <v>390</v>
-      </c>
       <c r="D14" s="17" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>404</v>
+      </c>
+      <c r="C16" t="s">
         <v>403</v>
       </c>
-      <c r="C16" t="s">
-        <v>402</v>
-      </c>
       <c r="D16" s="17" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
+        <v>407</v>
+      </c>
+      <c r="C18" t="s">
         <v>406</v>
       </c>
-      <c r="C18" t="s">
-        <v>405</v>
-      </c>
       <c r="D18" s="17" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
+        <v>431</v>
+      </c>
+      <c r="C20" t="s">
         <v>430</v>
       </c>
-      <c r="C20" t="s">
-        <v>429</v>
-      </c>
       <c r="D20" s="17" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
+        <v>454</v>
+      </c>
+      <c r="C22" t="s">
         <v>453</v>
       </c>
-      <c r="C22" t="s">
-        <v>452</v>
-      </c>
       <c r="D22" s="17" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C24" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="C25" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -6020,17 +5812,17 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -6167,18 +5959,18 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>457</v>
+      </c>
+      <c r="C16" t="s">
         <v>456</v>
-      </c>
-      <c r="C16" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>475</v>
+      </c>
+      <c r="C17" t="s">
         <v>474</v>
-      </c>
-      <c r="C17" t="s">
-        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -6270,18 +6062,18 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C4" t="s">
         <v>420</v>
-      </c>
-      <c r="C4" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>437</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>436</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed the broken links, the early FB articles i did  have messed up pictures in their html, thay all go to a bib pic, so be careful if u need to update one
</commit_message>
<xml_diff>
--- a/FB Posts.xlsx
+++ b/FB Posts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="17540" tabRatio="868"/>
+    <workbookView xWindow="16680" yWindow="0" windowWidth="19440" windowHeight="17540" tabRatio="868"/>
   </bookViews>
   <sheets>
     <sheet name="FB Posts" sheetId="1" r:id="rId1"/>
@@ -2798,9 +2798,9 @@
   <dimension ref="A1:T174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="660" topLeftCell="A112" activePane="bottomLeft"/>
+      <pane ySplit="660" topLeftCell="A118" activePane="bottomLeft"/>
       <selection activeCell="K1" sqref="K1:K1048576"/>
-      <selection pane="bottomLeft" activeCell="J112" sqref="J112"/>
+      <selection pane="bottomLeft" activeCell="M127" sqref="M127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0"/>
@@ -4832,6 +4832,9 @@
       <c r="K112" s="12" t="s">
         <v>345</v>
       </c>
+      <c r="M112" s="5">
+        <v>1</v>
+      </c>
       <c r="O112" s="3" t="s">
         <v>344</v>
       </c>
@@ -5002,7 +5005,7 @@
         <v>372</v>
       </c>
       <c r="M122" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O122" s="3" t="s">
         <v>716</v>
@@ -5025,7 +5028,7 @@
         <v>374</v>
       </c>
       <c r="M123" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O123" s="3" t="s">
         <v>375</v>
@@ -5085,7 +5088,7 @@
         <v>388</v>
       </c>
       <c r="M126" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O126" s="3" t="s">
         <v>387</v>
@@ -5128,7 +5131,7 @@
         <v>397</v>
       </c>
       <c r="M128" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q128" s="21" t="s">
         <v>396</v>
@@ -5182,7 +5185,7 @@
         <v>410</v>
       </c>
       <c r="M131" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O131" s="3" t="s">
         <v>409</v>
@@ -5236,7 +5239,7 @@
         <v>418</v>
       </c>
       <c r="M134" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O134" s="3" t="s">
         <v>416</v>
@@ -5256,7 +5259,7 @@
         <v>422</v>
       </c>
       <c r="M135" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q135" s="23" t="s">
         <v>421</v>
@@ -5293,7 +5296,7 @@
         <v>426</v>
       </c>
       <c r="M137" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O137" s="3" t="s">
         <v>427</v>
@@ -5390,7 +5393,7 @@
         <v>446</v>
       </c>
       <c r="M142" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q142" s="21" t="s">
         <v>445</v>
@@ -5576,7 +5579,7 @@
         <v>477</v>
       </c>
       <c r="M151" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O151" s="3" t="s">
         <v>476</v>
@@ -5596,7 +5599,7 @@
         <v>480</v>
       </c>
       <c r="M152" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O152" s="3" t="s">
         <v>677</v>

</xml_diff>

<commit_message>
Finished the grooming resources
</commit_message>
<xml_diff>
--- a/FB Posts.xlsx
+++ b/FB Posts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="19440" windowHeight="17540" tabRatio="868"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="868"/>
   </bookViews>
   <sheets>
     <sheet name="FB Posts" sheetId="1" r:id="rId1"/>
@@ -2798,9 +2798,9 @@
   <dimension ref="A1:T174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="660" topLeftCell="A118" activePane="bottomLeft"/>
+      <pane ySplit="660" topLeftCell="A2" activePane="bottomLeft"/>
       <selection activeCell="K1" sqref="K1:K1048576"/>
-      <selection pane="bottomLeft" activeCell="M127" sqref="M127"/>
+      <selection pane="bottomLeft" activeCell="Q140" sqref="Q140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Working on organizing the grooming resource
</commit_message>
<xml_diff>
--- a/FB Posts.xlsx
+++ b/FB Posts.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="868"/>
+    <workbookView xWindow="13080" yWindow="0" windowWidth="15540" windowHeight="16060" tabRatio="868" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FB Posts" sheetId="1" r:id="rId1"/>
-    <sheet name="Testimonials" sheetId="2" r:id="rId2"/>
-    <sheet name="Top Picks" sheetId="3" r:id="rId3"/>
-    <sheet name="Reading Pics" sheetId="4" r:id="rId4"/>
-    <sheet name="Barns" sheetId="5" r:id="rId5"/>
-    <sheet name="Art Horses" sheetId="6" r:id="rId6"/>
-    <sheet name="Instagram" sheetId="7" r:id="rId7"/>
-    <sheet name="x" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
+    <sheet name="Testimonials" sheetId="2" r:id="rId3"/>
+    <sheet name="Top Picks" sheetId="3" r:id="rId4"/>
+    <sheet name="Reading Pics" sheetId="4" r:id="rId5"/>
+    <sheet name="Barns" sheetId="5" r:id="rId6"/>
+    <sheet name="Art Horses" sheetId="6" r:id="rId7"/>
+    <sheet name="Instagram" sheetId="7" r:id="rId8"/>
+    <sheet name="x" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FB Posts'!$A$3:$T$156</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="1000">
   <si>
     <t>Link</t>
   </si>
@@ -2180,13 +2181,966 @@
   </si>
   <si>
     <t>Fbatman</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>SECTION</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>Listed/Resource As</t>
+  </si>
+  <si>
+    <t>Published by</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>Date/Issue/Vol.</t>
+  </si>
+  <si>
+    <t>Tags  (these should be keyword-rich)</t>
+  </si>
+  <si>
+    <t>Article Categories</t>
+  </si>
+  <si>
+    <t>Description / Summary (use if first sentance isn't keyword rich or descriptive)</t>
+  </si>
+  <si>
+    <t>Word Doc file name</t>
+  </si>
+  <si>
+    <t>flickr albumns url</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/TurnoutTips-p1.pdf</t>
+  </si>
+  <si>
+    <t>Turnout Tips 1</t>
+  </si>
+  <si>
+    <t>State of the Art</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/TurnoutTips-p2.pdf</t>
+  </si>
+  <si>
+    <t>Turnout Tips 2</t>
+  </si>
+  <si>
+    <t>MONDAY</t>
+  </si>
+  <si>
+    <t>Stable Management, Grooming</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/BlanketRules.pdf</t>
+  </si>
+  <si>
+    <t>Blanketing Rules</t>
+  </si>
+  <si>
+    <t>Salt Block Gazette</t>
+  </si>
+  <si>
+    <t>horse, care, horsemanship, cooler, grooming, leg, straps, show, horse, pony, surcingle, sheet, safety, ruthann smith, lucky braids, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t>Safety &amp; soundness concerns for your equine may be suprising, too.</t>
+  </si>
+  <si>
+    <t>Grooming</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/CurryGHJ.pdf</t>
+  </si>
+  <si>
+    <t>CURRY! Groom to Listen</t>
+  </si>
+  <si>
+    <t>Gypsy Horse Journal</t>
+  </si>
+  <si>
+    <t>Grooming Kit</t>
+  </si>
+  <si>
+    <t>groom, curry, soundness, horse, care, gypsy, horse, show, soundness, ruthann smith, lucky braids, top turnout rubbing, itching</t>
+  </si>
+  <si>
+    <t>Groom your horse for soundness, health &amp; top turnout.</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/DressforBed.pdf</t>
+  </si>
+  <si>
+    <t>Dress for Bed</t>
+  </si>
+  <si>
+    <t>Equine Journal</t>
+  </si>
+  <si>
+    <t>grooming, horse, care, shampoo, rubs, safety, sheet, cooler, moving, blankets, hair, breakage, groom, strap, surcingle</t>
+  </si>
+  <si>
+    <t>Clothe horses for safety, soundness &amp; success under saddle.</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/ClothingForWork.pdf</t>
+  </si>
+  <si>
+    <t>Dress for Work</t>
+  </si>
+  <si>
+    <t>grooming, horse, care, quarter, sheet, safety, cooler, riding, soundness, equine, pony, ride, kidney, back, wool, fleece, ruthann</t>
+  </si>
+  <si>
+    <t>Cold bodies get injured.  Instead, promote soundness.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://luckybraids.com/edu/feathered-feet.pdf </t>
+  </si>
+  <si>
+    <t>Feathered Foot Care</t>
+  </si>
+  <si>
+    <t>horse shampoo, feather, hoof, white, gypsy horse, draft horse, thrush, mites</t>
+  </si>
+  <si>
+    <t>Horses' feathers can protect skin, but also exasperate problems. Here are tips to caring for the feathers hoof.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://www.chronofhorse.com/article/tack-room-ruthann-smith</t>
+    </r>
+  </si>
+  <si>
+    <t>Grooming Q &amp; A</t>
+  </si>
+  <si>
+    <t>Chronicle of the Horse</t>
+  </si>
+  <si>
+    <t>mane, pull, tail, rub, braid, braider, roach, body, clip, tails, stains, chestnut, coat, winter, thick, ruthann, smith, lucky braids, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t>Are you at a loss with your horse's mane, tail or coat?  Ruthann addresses pervasive grooming problems.</t>
+  </si>
+  <si>
+    <t>Manes &amp; Tails, Grooming</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/Farmvet-Catalogue-TAIL-TIPS.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Tail Care </t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Farmvet.com</t>
+  </si>
+  <si>
+    <t>horse, shampoo, hair,  breakage, bathing, grooming, tail, urine, stain, whitener, whitening, farmvet, lucky braids, top turnout, turn-out, groom, show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven best practices for big, healthy tails that are even easy to manage.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://luckybraids.com/edu/TallTails.pdf </t>
+  </si>
+  <si>
+    <t>Tall Tails</t>
+  </si>
+  <si>
+    <t>horse shampoo, hair breakage, bathing, grooming, tail, urine, stain</t>
+  </si>
+  <si>
+    <t>Conventional horse care promotes tail breakage.  Here's how to get the fullest tails naturally.</t>
+  </si>
+  <si>
+    <t>Stable Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://luckybraids.com/edu/KeenHorsemen.pdf </t>
+  </si>
+  <si>
+    <t>Keen Horsemen</t>
+  </si>
+  <si>
+    <t>sound, horsemanship, soundness, grooming, horse, care, training, awareness, peter wylde, ruthann smith, lucky braids, clinic, top turnout</t>
+  </si>
+  <si>
+    <t>Some consider it fashionable to know a lot.  True horsemen don't.</t>
+  </si>
+  <si>
+    <t>Big Tails</t>
+  </si>
+  <si>
+    <t>Skin</t>
+  </si>
+  <si>
+    <t>Glistening Greys</t>
+  </si>
+  <si>
+    <t>Braiding Beautifully</t>
+  </si>
+  <si>
+    <t>07_28_14</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/ManePrepWeb.pdf</t>
+  </si>
+  <si>
+    <t>Mane Prepping</t>
+  </si>
+  <si>
+    <t>groom, mane, pull, mane, train, horse, care, horsemanship, show, shampoo, braid, braider, ruthann smith, equestrian, festival, lucky braids, top, turnout, turn-out, pony, hunter, show, jumper, equitation, lucky braids, horse, shampoo</t>
+  </si>
+  <si>
+    <t>Conventional horse care is wrought with myth.  Here are best practices for crafting and maintaining manes.</t>
+  </si>
+  <si>
+    <t>Grooming, Stable Management</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/BatheForSoundness.pdf</t>
+  </si>
+  <si>
+    <t>Bathing for Soundness</t>
+  </si>
+  <si>
+    <t>horse, shampoo, scratches, crud, heel, leg, lameness, soundness, fungus, groom, show, bath, sound, cold, back, ruthann, smith, lucky braids, all-in-one</t>
+  </si>
+  <si>
+    <t>Improper bathing can lead to soreness, insecurity and even death.  No kidding.</t>
+  </si>
+  <si>
+    <t>Braiding, Manes &amp; Tails</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/pdf/State-of-the-Art.pdf</t>
+  </si>
+  <si>
+    <t>Braiding: State of the Art</t>
+  </si>
+  <si>
+    <t>LuckyBraids.com</t>
+  </si>
+  <si>
+    <t>George Morris, micheal matz, peter wylde, mane, braid, braider,  tail, dressage, hunter, equitation, groom, Micheal Matz, lucky braids, top turnout, ruthann smith, pro</t>
+  </si>
+  <si>
+    <t>A good braid job can improve your performance for a lot of reasons.  Here's what the top pros attest.</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/buff-braiding_PH1107.pdf</t>
+  </si>
+  <si>
+    <t>Buff Up Braiding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Plaid Horse </t>
+  </si>
+  <si>
+    <t>braid, mane, pro, braider, groom, show, dressage, hunter, dressage, equitation, lucky braids, top, turnout, turn-out, ruthann, smith</t>
+  </si>
+  <si>
+    <t>Learn Ruthann's braiding formula to braid any horse beautifully, comfortably and quickly.</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/ManeTaming.pdf</t>
+  </si>
+  <si>
+    <t>Mane Taming</t>
+  </si>
+  <si>
+    <t>big, thick, mane, tame, groom, show, top turnout, horse, train, braider, braid, pull, horsemanship, turnout, turn-out, Ruthann, shampoo, lucky braids</t>
+  </si>
+  <si>
+    <t>Mane unruly?  It just needs these best practices for top turnout.</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/ScratchesGHJgroom.pdf</t>
+  </si>
+  <si>
+    <t>Scrap Scratches</t>
+  </si>
+  <si>
+    <t>scratches, fungus, crud, horse, shampoo, groom, care, soundness, lameness, horse, pony cob, gypsy, feather, ruthann, smith, lucky braids, top, turn-out, turnout</t>
+  </si>
+  <si>
+    <t>A little crud can lead to lameness and a systemic infection.  Here's how to get and keep out of the loop.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>LOW REZ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://www.luckybraids.com/pdf/GroomingTipsDateline.pdf</t>
+    </r>
+  </si>
+  <si>
+    <t>Grooming Tips</t>
+  </si>
+  <si>
+    <t>safety, groom, horse, bathing, horse, shampoo, pony, stain, tail, whitening, handling, safety, ruthann, smith, horsemanship, care</t>
+  </si>
+  <si>
+    <t>Grooming routines can save you time and money in the barn and at horse shows.</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/CrosstieEtiquette.pdf</t>
+  </si>
+  <si>
+    <t>Crosstie Ettiquette</t>
+  </si>
+  <si>
+    <t>Safety,  grooming, horse show, breakaway, break-away, time, stable, management, crosstie, cross-tie, leading, tying, horse, cross, tie, aisle, barn, safety, ruthann, smith</t>
+  </si>
+  <si>
+    <t>Accidents wait to happen.  Everyday accidents wait to happen.
+Etiquette is a matter of safety.</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/DressageTurnout.pdf</t>
+  </si>
+  <si>
+    <t>Dressage Turnout</t>
+  </si>
+  <si>
+    <t>braid, dressage, groom, horse, show, pull, tail, button, dutch, braider, ruthann, smith, lucky braids, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t>Earn the judges' respect with proper turnout.</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/drink-up.pdf</t>
+  </si>
+  <si>
+    <t>Drink Up</t>
+  </si>
+  <si>
+    <t>horse, hydration, hydrate, drink, ship, show, ride, hot, heat, colic, pony, ship, trailer, ruthann, smith, lucky braids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keeping your horse hydrated is pivotal to every aspect of his well-being and performance. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Manes &amp; Tails</t>
+  </si>
+  <si>
+    <t>http://www.equisearch.com/article/eqsmithcha673</t>
+  </si>
+  <si>
+    <t>Mane &amp; Tail Chat</t>
+  </si>
+  <si>
+    <t>Equisearch.com</t>
+  </si>
+  <si>
+    <t>braid, mane, braider, tail, thick, cresty, flat, button, dressage, jumper, hunter, draft, ruthann, smith, lucky braids, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t>Every wonder how braids can be so perfect? Ruthann shares techniques for tricky manes and tails.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sat Aug 2 </t>
+  </si>
+  <si>
+    <t>Stable Mangement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the Environment &amp; Soundness </t>
+  </si>
+  <si>
+    <t>stall, bed, shavings, soundness, management, stable, care, horse, groom, ruthann, smith, lucky braids, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand the impact of your choices on not only the environment but also horses’ soundness.  </t>
+  </si>
+  <si>
+    <t>stall, bedding, shavings, soundness, management, horse, equine, journal, groom, ruthann, smith,  horsemanship, save, conserve, green</t>
+  </si>
+  <si>
+    <t>Braiding</t>
+  </si>
+  <si>
+    <t>Ruthann's Braiding Formula Tips</t>
+  </si>
+  <si>
+    <t>PR Web</t>
+  </si>
+  <si>
+    <t>braid, braider, mane, groom, horses, equine, equestrian, show, top, turnout, turn-out, ruthann, smith, formula, yarn, lucky braids</t>
+  </si>
+  <si>
+    <t>Braiding is like salsa dancing. Its easy when you know the moves. Here are some steps…</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/pdf/GreenGrooming.pdf</t>
+  </si>
+  <si>
+    <t>Green Grooming</t>
+  </si>
+  <si>
+    <t>horse, conservation, grooming, management, husbandry, care, stable, bedding, conserve, ruthann, smith, lucky braids, all-in-one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have you considered that global warming, allergies and cancer all seem to point to toxins?  </t>
+  </si>
+  <si>
+    <t>Ruthann, Grooming, Braiding</t>
+  </si>
+  <si>
+    <t>Braiding was Just Ruthann's Start</t>
+  </si>
+  <si>
+    <t>ruthann, braid, pro, groom, entreprenuer, braider, horse, show, pony, horsemanship, care, husbandry, lucky braids, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When Ruthann Smith first climbed onto a ladder to braid her pony at age 8, she never imagined where those steps would take her.  </t>
+  </si>
+  <si>
+    <t>Ruthann, Braiding</t>
+  </si>
+  <si>
+    <t>Ruthann At the Back Gate</t>
+  </si>
+  <si>
+    <t>Gait Post</t>
+  </si>
+  <si>
+    <t>ruthann, smith, braiding, braider, groom, entreprenuer, show, coat, care, DVD, video, pro, horsemanship, clinic, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t>Smith has dedicated herself to improving the lives of horses by raising the bar of turnout, daily care and handling.</t>
+  </si>
+  <si>
+    <t>Braiding, Ruthann</t>
+  </si>
+  <si>
+    <t>http://www.prweb.com/printer/310911.htm</t>
+  </si>
+  <si>
+    <t>Braiding Secrets Revealed (SAME AS SECRETS)</t>
+  </si>
+  <si>
+    <t>ruthann, braiding, grooming, how-to, braider, horse show, video, DVD, tools, yarn, lucky braids, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t>Imagine if braiding could be quick, comfortable and consistenly gorgeous.</t>
+  </si>
+  <si>
+    <t>Martha Stewart of Braiding</t>
+  </si>
+  <si>
+    <t>Equestrian Retailer</t>
+  </si>
+  <si>
+    <t>ruthann, smith, braid, grooming, how-to, braider, horse, show, video, DVD, tools, yarn, lucky braids, top, turnout, turn-out, pro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Braiding can be a gateway to a holistic approach to horse care that begins with beautiful braids and ends with a happier, healthier, more relaxed horse-and-rider team. 
+Braids and Top Turnout Inc., 
+braiding isn't just another 
+frustrating item on a 
+pre-show checklist, but the gateway 
+to a holistic approach to horse care 
+that begins with beautiful braids 
+and ends with a happier, healthier, 
+more relaxed horse-and-rider team. 
+Ruthann Smith of Lucky 
+Braids and Top Turnout Inc., 
+braiding isn't just another 
+frustrating item on a 
+pre-show checklist, but the gateway 
+to a holistic approach to horse care 
+that begins with beautiful braids 
+and ends with a happier, healthier, 
+more relaxed horse-and-rider team. 
+Ruthann Smith of Lucky 
+Braids and Top Turnout Inc., 
+braiding isn't just another 
+frustrating item on a 
+pre-show checklist, but the gateway 
+to a holistic approach to horse care 
+that begins with beautiful braids 
+and ends with a happier, healthier, 
+more relaxed horse-and-rider team. 
+Ruthann Smith of Lucky 
+Braids and Top Turnout Inc., 
+braiding isn't just another 
+frustrating item on a 
+pre-show checklist, but the gateway 
+to a holistic approach to horse care 
+that begins with beautiful braids 
+and ends with a happier, healthier, 
+more relaxed horse-and-rider team. 
+Ruthann Smith of Lucky 
+Braids and Top Turnout Inc., 
+braiding isn't just another 
+frustrating item on a 
+pre-show checklist, but the gateway 
+to a holistic approach to horse care 
+that begins with beautiful braids 
+and ends with a happier, healthier, 
+more relaxed horse-and-rider team. 
+braiding isn't just another 
+frustrating item on a 
+pre-show checklist, but the gateway 
+to a holistic approach to horse care 
+that begins with beautiful braids 
+and ends with a happier, healthier, 
+more relaxed horse-and-rider team. 
+braiding isn't just another 
+frustrating item on a 
+pre-show checklist, but the gateway 
+to a holistic approach to horse care 
+that begins with beautiful braids 
+and ends with a happier, healthier, 
+more relaxed horse-and-rider team. 
+</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/stain-Less.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stain Less </t>
+  </si>
+  <si>
+    <t xml:space="preserve">groom, stain, grey, gray, white, horse, show, care, urine, manure, sock, tail, shampoo, all-in-one, lucky braids, ruthann, turnout, cowboy magic, </t>
+  </si>
+  <si>
+    <t>Here's how grooming greys can be stain free and easy.</t>
+  </si>
+  <si>
+    <t>Sun Bleaching</t>
+  </si>
+  <si>
+    <t>sun, bleaching, burn, groom, horse, all-in-one, shampoo, bug, summer, care, pony, pasture, lucky braids, top, turnout, turn-out, gypsy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are lots of things that can minimize the sun’s impact on a horse’s coat. </t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/TackTrack.pdf</t>
+  </si>
+  <si>
+    <t>Tack Track</t>
+  </si>
+  <si>
+    <t>groom, saddle, bridle, cleaning, leather, horse, care, clean, soap, oil, horsemanship, stable, barn, ruthann, smith, lucky braids, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t>Here are some quick cost-saving tips that also impress the horse show judges.</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/TimeManagementGroomingStalls.pdf</t>
+  </si>
+  <si>
+    <t>Time Management</t>
+  </si>
+  <si>
+    <t>groom, horse, show, horse, care, win, management, stable, ruthann, smith, sound, horsemanship, lucky braids, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time management is fundamental to sound horsemanship. </t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/UrinatingOutsideStalls.pdf</t>
+  </si>
+  <si>
+    <t>Urinating Outside</t>
+  </si>
+  <si>
+    <t>horse, care, stable, urinate, show, groom, horsemanship, management, stable, barn, ruthann, smith, equine, journal, pony, lucky braids, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t>This article outlines what impacts your horse’s health and performance as well as recommended routines.</t>
+  </si>
+  <si>
+    <t>Wed Aug 6</t>
+  </si>
+  <si>
+    <t>grooming, safety</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/pdf/BathingFaces.pdf</t>
+  </si>
+  <si>
+    <t>Bathing Faces</t>
+  </si>
+  <si>
+    <t>bathing, face, head, horse, care, safety, wash, horse, groom, care, shampoo, lucky braids, horsemanship, top turnout, turn-out</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/TopTurnoutSBG-coatcare.pdf</t>
+  </si>
+  <si>
+    <t>Big Hearts Win</t>
+  </si>
+  <si>
+    <t>show sheen, tail, care, shine, ears, trim, clip, hoof, fit, tack, scratches, crud, fungus, detangler, bridlepath, lucky braids, top turnout</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/pdf/NippedNose.pdf</t>
+  </si>
+  <si>
+    <t>Buckets &amp; Snaps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">safety, barn, bucket, snap, nostril, stable, management, horse, care, husbandry, ruthann, smith, lucky braids, equine, journal </t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/pdf/Circulation.pdf</t>
+  </si>
+  <si>
+    <t>Circulation</t>
+  </si>
+  <si>
+    <t>Holistic Horse</t>
+  </si>
+  <si>
+    <t>groom, horse, equine, curry, towel, care, horse, health, holistic, pony, currying, lucky braids, top turnout, turn-out, shine</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/TallTails.pdf</t>
+  </si>
+  <si>
+    <t>Care for Big Tails</t>
+  </si>
+  <si>
+    <t>tail, care, horse, tail, breakage, growth, groom, braid, braider, show sheen, detangler, cowboy magic, lucky braids, ruthann, top turnout</t>
+  </si>
+  <si>
+    <t>management, safety</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/pdf/CrossTie1.pdf **AND** http://www.luckybraids.com/pdf/CrossTie2.pdf</t>
+  </si>
+  <si>
+    <t>Crosstie Myths &amp; Safety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barn, safety, stall, horse, care, horsemanship, ruthann, dmith, stable, management, lucky braids, top turnout, show, equestrian </t>
+  </si>
+  <si>
+    <t>grooming, handling, safety</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/pdf/HalterFit.pdf *AND* http://www.luckybraids.com/pdf/HalterFit2.pdf</t>
+  </si>
+  <si>
+    <t>Halter Fit</t>
+  </si>
+  <si>
+    <t>halter, horse, equine, pony, fit, leading, safety, horsesmanship, sound, horsemanship, top turnout, equestrian, accident, equine, ruthann</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/pdf/HoofTips.pdf</t>
+  </si>
+  <si>
+    <t>Holistic Hoof Tips</t>
+  </si>
+  <si>
+    <t>hoof, care, thrush, horse, lucky braids, paint, sole, pack, feet, horsemanship, groom, footing, ruthann, smith, soundness, horsemanship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.luckybraids.com/pdf/Leading%201_2EJ%20Aug07.pdf *AND* http://www.luckybraids.com/pdf/Leading%202_2EJAug07.pdf </t>
+  </si>
+  <si>
+    <t>Safe Leading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horsemanship, sound, horse, care, handling, lucky braids, safety, ruthann, smith, lead, shank, rope, </t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/nix-scratches.pdf</t>
+  </si>
+  <si>
+    <t>Nix Scratches</t>
+  </si>
+  <si>
+    <t>grooming, management</t>
+  </si>
+  <si>
+    <t>Product of Year</t>
+  </si>
+  <si>
+    <t>Horse Journal</t>
+  </si>
+  <si>
+    <t>horse, shampoo, stain, remover, whitening, medicated, lucky braids, whitener, all-in-one, rinse, condition, award-winning, equine, journal</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/pdf/PullingDemystified.pdf</t>
+  </si>
+  <si>
+    <t>Pulling Demystified</t>
+  </si>
+  <si>
+    <t>?????</t>
+  </si>
+  <si>
+    <t>Ride! Magazine</t>
+  </si>
+  <si>
+    <t>pull, mane, thick, braid, braider, shortening, lucky braids, ruthann, smith, handling, solo comb, technique, how-to, horsemanship, husbandry</t>
+  </si>
+  <si>
+    <t>Mt</t>
+  </si>
+  <si>
+    <t>http://www.chronofhorse.com/Images/0506PullingTips.pdf</t>
+  </si>
+  <si>
+    <t>Pulling Peacefully</t>
+  </si>
+  <si>
+    <t>Chronofhorse.com</t>
+  </si>
+  <si>
+    <t>pull, mane, thick, hate, handling, peaceful, lucky braids, solo, comb, groom, show, braid, braider, ruthann, smith, lucky braids</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/rubs.pdf</t>
+  </si>
+  <si>
+    <t>Rubs</t>
+  </si>
+  <si>
+    <t>horse, shampoo, blanket, boot, rub, groom, shampoo, pony, shoulder, leg, care, sheet, winter, care, ruthann, smith, equine, lucky braids, top turnout, turn-out</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/grooming-articles.htm</t>
+  </si>
+  <si>
+    <t>Stretch</t>
+  </si>
+  <si>
+    <t>stretch, legs, saddle, girth, grooming, sore, horse, care, lucky braids, top turnout, turno-out, dressage, jumper, show, horsemanship, equine, journal</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/pdf/Nix_Tail_Rubbing.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tail Rubbing </t>
+  </si>
+  <si>
+    <t>horse, shampoo, tail, rub, rubbing, handy, salve, itching, calm coat, braiding, lucky Braids, ruthann, horse care, grooming</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/erase-stains-HorseJournal0308.pdf</t>
+  </si>
+  <si>
+    <t>Top Pick to Erase Stains</t>
+  </si>
+  <si>
+    <t>horse, shampoo, grey, stain, sock, urine, manure, horse care, whitener, remover, cowboy magic, quick silver, bluing, lucky braids, hock</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/clinics.htm</t>
+  </si>
+  <si>
+    <t>Top Turnout Clinics</t>
+  </si>
+  <si>
+    <t>ruthann, smith, lucky braids, top turnout, turn-out, groom, horse, all-in-one, shampoo, care, handling, safety, horsemanship, clinic, husbandry, equine</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/pdf/TrimmingTips.pdf</t>
+  </si>
+  <si>
+    <t>Trimming Tips</t>
+  </si>
+  <si>
+    <t>clip, trim, ear, muzzle, horse, care, lucky braids, top turnout, turn-out, ruthann, smith, line, cold, eye, eyelash, wisker, horsemanship, show</t>
+  </si>
+  <si>
+    <t>braiding, Ruthann</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/video-promo.html</t>
+  </si>
+  <si>
+    <t>Video Samples</t>
+  </si>
+  <si>
+    <t>braid, hunter, jumper dressage, driving, horse, lucky braids, grooming, show, ruthann, smith, braider, horsemanship, equitation, junior</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/WhiteLies.pdf</t>
+  </si>
+  <si>
+    <t>White Lies</t>
+  </si>
+  <si>
+    <t>horse, shampoo, stain, remover, whitener, whitening, shine, grey, white, gray, tail, hock, pony, ponies, lucky braids, ruthann, cowboy magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> management</t>
+  </si>
+  <si>
+    <t>Winter Wisdom</t>
+  </si>
+  <si>
+    <t>horse, groom, winter, hydration, grooming, care, tack, ruthann, smith, husbandry, horsemanship, winter, cold, colic</t>
+  </si>
+  <si>
+    <t>testtimonials</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/testimonials.pdf</t>
+  </si>
+  <si>
+    <t>Word on the Aisle</t>
+  </si>
+  <si>
+    <t>molly ashe, kim prince, ian millar, jefferey welles, micheal matz, horse, shampoo, salve, whitener, skin disease, fungus, crud, lucky braids, groom, show sheen</t>
+  </si>
+  <si>
+    <t>RUTHANN</t>
+  </si>
+  <si>
+    <t>Ruthann, braiding</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/edu/back-gate.pdf</t>
+  </si>
+  <si>
+    <t>Back Gate</t>
+  </si>
+  <si>
+    <t>The Gait Post</t>
+  </si>
+  <si>
+    <t>ruthann, smith, groom, braid, braider, horse, shampoo, clinic, lucky braids, top, turnout, turn-out, tail, mane,  dvd, video, horsemanship, clinic, quik braid</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/pdf/RSmith-071803.pdf</t>
+  </si>
+  <si>
+    <t>Braiding was the Start</t>
+  </si>
+  <si>
+    <t>chronofhorse, chronicle, horse, equine, braid, braider, Ruthann, groom, care, show, hunter, lucky braids, top, turnout, turn-out, dressage, george morris</t>
+  </si>
+  <si>
+    <t>Braiding Tips</t>
+  </si>
+  <si>
+    <t>Plaid Horse</t>
+  </si>
+  <si>
+    <t>braid, braider, mane, tail, ruthann, smith, lucky braids, yarn, cramp, hand, dvd, learn, professional, turn-out, quik braid, formula, top, turnout, turn-out</t>
+  </si>
+  <si>
+    <t>Big Hair</t>
+  </si>
+  <si>
+    <t>gypsy, horse, mane, tail, hair, breakage, braid, care, groom, shampoo, stain, whitener, show sheen, cowboy magic, long, thick, horsemanship, groom</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/pdf/BedGreen1.pdf</t>
+  </si>
+  <si>
+    <t>Bed Green 1</t>
+  </si>
+  <si>
+    <t>groom, horse, care, equine, shavings, bedding, pellets, stall, lucky braids, clean, conserve, save, journal, husbandry, horsemanship, ruthann, smith, lucky braids</t>
+  </si>
+  <si>
+    <t>http://luckybraids.com/pdf/BedGreen2.pdf</t>
+  </si>
+  <si>
+    <t>Bed Green 2</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/edu/ClippingPivotPoints.pdf</t>
+  </si>
+  <si>
+    <t>Clip Tips</t>
+  </si>
+  <si>
+    <t>clip, trim, body, clippers, equine, turnout, turn-out, lines, winter, grooming, show, horse, care, Ruthann, smith, lucky braids, show, trace</t>
+  </si>
+  <si>
+    <t>http://www.luckybraids.com/pdf/SafeHorseBlanketHandling.pdf</t>
+  </si>
+  <si>
+    <t>Blanketing Safety</t>
+  </si>
+  <si>
+    <t>horse, care, safey, pony, blanket, sheet, clothing, grooming, move, turnout, rug, ruthann, lucky braids, rub, cold, move, horsemanship, stable, stablewear</t>
+  </si>
+  <si>
+    <t>mT</t>
+  </si>
+  <si>
+    <t>pull, mane, blade, comb, shorten, ruthann, smith, lucky braids, show, dressage, jumper, braidable, horse, crest, thick, big, pony, cut, technique</t>
+  </si>
+  <si>
+    <t>Bed Green</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Bedding Myths (OMIT_ Same As Bedding green</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2303,8 +3257,153 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF231F20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF231F20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2371,6 +3470,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCECFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2390,15 +3513,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2492,11 +3620,134 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="19" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="21" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="25" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="25" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="25" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2797,10 +4048,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="660" topLeftCell="A2" activePane="bottomLeft"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="660" topLeftCell="A143" activePane="bottomLeft"/>
       <selection activeCell="K1" sqref="K1:K1048576"/>
-      <selection pane="bottomLeft" activeCell="Q140" sqref="Q140"/>
+      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0"/>
@@ -5869,6 +7120,1809 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A29" activePane="bottomLeft"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
+      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="16.75" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" style="60" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="60" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" style="60" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="60" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="60" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="60" customWidth="1"/>
+    <col min="7" max="7" width="19.5" style="60" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" style="91" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="60" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="2.5" style="60" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="60" customWidth="1"/>
+    <col min="12" max="13" width="18.33203125" style="60" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="127.83203125" style="60" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="60" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="44.1640625" style="60" customWidth="1"/>
+    <col min="17" max="18" width="18.33203125" style="60" hidden="1" customWidth="1"/>
+    <col min="19" max="16384" width="17.33203125" style="60"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A1" s="55" t="s">
+        <v>717</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55" t="s">
+        <v>718</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>719</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="58" t="s">
+        <v>720</v>
+      </c>
+      <c r="J1" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="58" t="s">
+        <v>721</v>
+      </c>
+      <c r="L1" s="59" t="s">
+        <v>722</v>
+      </c>
+      <c r="M1" s="58" t="s">
+        <v>723</v>
+      </c>
+      <c r="N1" s="58" t="s">
+        <v>724</v>
+      </c>
+      <c r="O1" s="58" t="s">
+        <v>725</v>
+      </c>
+      <c r="P1" s="58" t="s">
+        <v>726</v>
+      </c>
+      <c r="Q1" s="58" t="s">
+        <v>727</v>
+      </c>
+      <c r="R1" s="55" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="61"/>
+    </row>
+    <row r="3" spans="1:18" s="73" customFormat="1" ht="16.75" customHeight="1">
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="69" t="s">
+        <v>729</v>
+      </c>
+      <c r="H3" s="70" t="s">
+        <v>730</v>
+      </c>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71" t="s">
+        <v>731</v>
+      </c>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="67"/>
+    </row>
+    <row r="4" spans="1:18" s="73" customFormat="1" ht="16.75" customHeight="1">
+      <c r="A4" s="67"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="69" t="s">
+        <v>732</v>
+      </c>
+      <c r="H4" s="70" t="s">
+        <v>733</v>
+      </c>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="67"/>
+    </row>
+    <row r="5" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A5" s="74"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="75" t="s">
+        <v>734</v>
+      </c>
+      <c r="G5" s="74"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
+      <c r="R5" s="74"/>
+    </row>
+    <row r="6" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A6" s="74"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="79" t="s">
+        <v>735</v>
+      </c>
+      <c r="G6" s="74" t="s">
+        <v>736</v>
+      </c>
+      <c r="H6" s="76" t="s">
+        <v>737</v>
+      </c>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77">
+        <v>1</v>
+      </c>
+      <c r="K6" s="77" t="s">
+        <v>738</v>
+      </c>
+      <c r="M6" s="78"/>
+      <c r="N6" s="77" t="s">
+        <v>739</v>
+      </c>
+      <c r="O6" s="77"/>
+      <c r="P6" s="77" t="s">
+        <v>740</v>
+      </c>
+      <c r="Q6" s="77"/>
+      <c r="R6" s="74"/>
+    </row>
+    <row r="7" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A7" s="74"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="79" t="s">
+        <v>741</v>
+      </c>
+      <c r="G7" s="74" t="s">
+        <v>742</v>
+      </c>
+      <c r="H7" s="76" t="s">
+        <v>743</v>
+      </c>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77">
+        <v>1</v>
+      </c>
+      <c r="K7" s="77" t="s">
+        <v>744</v>
+      </c>
+      <c r="L7" s="77" t="s">
+        <v>745</v>
+      </c>
+      <c r="M7" s="78"/>
+      <c r="N7" s="77" t="s">
+        <v>746</v>
+      </c>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77" t="s">
+        <v>747</v>
+      </c>
+      <c r="Q7" s="77"/>
+      <c r="R7" s="74"/>
+    </row>
+    <row r="8" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A8" s="74"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="79" t="s">
+        <v>735</v>
+      </c>
+      <c r="G8" s="80" t="s">
+        <v>748</v>
+      </c>
+      <c r="H8" s="76" t="s">
+        <v>749</v>
+      </c>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77">
+        <v>1</v>
+      </c>
+      <c r="K8" s="81" t="s">
+        <v>750</v>
+      </c>
+      <c r="L8" s="77"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="77" t="s">
+        <v>751</v>
+      </c>
+      <c r="O8" s="77"/>
+      <c r="P8" s="77" t="s">
+        <v>752</v>
+      </c>
+      <c r="Q8" s="77"/>
+      <c r="R8" s="74"/>
+    </row>
+    <row r="9" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A9" s="74"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="79" t="s">
+        <v>735</v>
+      </c>
+      <c r="G9" s="80" t="s">
+        <v>753</v>
+      </c>
+      <c r="H9" s="76" t="s">
+        <v>754</v>
+      </c>
+      <c r="I9" s="77"/>
+      <c r="J9" s="82">
+        <v>1</v>
+      </c>
+      <c r="K9" s="81" t="s">
+        <v>750</v>
+      </c>
+      <c r="L9" s="77"/>
+      <c r="M9" s="78"/>
+      <c r="N9" s="77" t="s">
+        <v>755</v>
+      </c>
+      <c r="O9" s="77"/>
+      <c r="P9" s="77" t="s">
+        <v>756</v>
+      </c>
+      <c r="Q9" s="77"/>
+      <c r="R9" s="74"/>
+    </row>
+    <row r="10" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A10" s="74"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="79" t="s">
+        <v>741</v>
+      </c>
+      <c r="G10" s="80" t="s">
+        <v>757</v>
+      </c>
+      <c r="H10" s="76" t="s">
+        <v>758</v>
+      </c>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77">
+        <v>1</v>
+      </c>
+      <c r="K10" s="77" t="s">
+        <v>744</v>
+      </c>
+      <c r="L10" s="77"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="77" t="s">
+        <v>759</v>
+      </c>
+      <c r="O10" s="77"/>
+      <c r="P10" s="77" t="s">
+        <v>760</v>
+      </c>
+      <c r="Q10" s="77"/>
+      <c r="R10" s="74"/>
+    </row>
+    <row r="11" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A11" s="74"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="79" t="s">
+        <v>741</v>
+      </c>
+      <c r="G11" s="74" t="s">
+        <v>761</v>
+      </c>
+      <c r="H11" s="76" t="s">
+        <v>762</v>
+      </c>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77">
+        <v>1</v>
+      </c>
+      <c r="K11" s="81" t="s">
+        <v>763</v>
+      </c>
+      <c r="L11" s="77"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="77" t="s">
+        <v>764</v>
+      </c>
+      <c r="O11" s="77"/>
+      <c r="P11" s="77" t="s">
+        <v>765</v>
+      </c>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="74"/>
+    </row>
+    <row r="12" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A12" s="74"/>
+      <c r="B12" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="79" t="s">
+        <v>766</v>
+      </c>
+      <c r="G12" s="74" t="s">
+        <v>767</v>
+      </c>
+      <c r="H12" s="76" t="s">
+        <v>768</v>
+      </c>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77" t="s">
+        <v>769</v>
+      </c>
+      <c r="K12" s="81" t="s">
+        <v>770</v>
+      </c>
+      <c r="L12" s="77"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="77" t="s">
+        <v>771</v>
+      </c>
+      <c r="O12" s="77"/>
+      <c r="P12" s="77" t="s">
+        <v>772</v>
+      </c>
+      <c r="Q12" s="77"/>
+      <c r="R12" s="74"/>
+    </row>
+    <row r="13" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A13" s="74"/>
+      <c r="B13" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="79" t="s">
+        <v>766</v>
+      </c>
+      <c r="G13" s="74" t="s">
+        <v>773</v>
+      </c>
+      <c r="H13" s="76" t="s">
+        <v>774</v>
+      </c>
+      <c r="I13" s="77"/>
+      <c r="J13" s="77">
+        <v>1</v>
+      </c>
+      <c r="K13" s="81" t="s">
+        <v>750</v>
+      </c>
+      <c r="L13" s="77"/>
+      <c r="M13" s="78"/>
+      <c r="N13" s="77" t="s">
+        <v>775</v>
+      </c>
+      <c r="O13" s="77"/>
+      <c r="P13" s="77" t="s">
+        <v>776</v>
+      </c>
+      <c r="Q13" s="77"/>
+      <c r="R13" s="74"/>
+    </row>
+    <row r="14" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="79" t="s">
+        <v>777</v>
+      </c>
+      <c r="G14" s="80" t="s">
+        <v>778</v>
+      </c>
+      <c r="H14" s="76" t="s">
+        <v>779</v>
+      </c>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77">
+        <v>1</v>
+      </c>
+      <c r="K14" s="81" t="s">
+        <v>750</v>
+      </c>
+      <c r="L14" s="77"/>
+      <c r="M14" s="78"/>
+      <c r="N14" s="77" t="s">
+        <v>780</v>
+      </c>
+      <c r="O14" s="77"/>
+      <c r="P14" s="77" t="s">
+        <v>781</v>
+      </c>
+      <c r="Q14" s="77"/>
+      <c r="R14" s="74"/>
+    </row>
+    <row r="15" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A15" s="74"/>
+      <c r="B15" s="74" t="s">
+        <v>782</v>
+      </c>
+      <c r="C15" s="74" t="s">
+        <v>783</v>
+      </c>
+      <c r="D15" s="74" t="s">
+        <v>784</v>
+      </c>
+      <c r="E15" s="74" t="s">
+        <v>785</v>
+      </c>
+      <c r="F15" s="79"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="78"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="77"/>
+      <c r="P15" s="77"/>
+      <c r="Q15" s="77"/>
+      <c r="R15" s="74"/>
+    </row>
+    <row r="16" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A16" s="74"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="75" t="s">
+        <v>786</v>
+      </c>
+      <c r="G16" s="74"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="77"/>
+      <c r="K16" s="77"/>
+      <c r="L16" s="77"/>
+      <c r="M16" s="78"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="77"/>
+      <c r="P16" s="77"/>
+      <c r="Q16" s="77"/>
+      <c r="R16" s="74"/>
+    </row>
+    <row r="17" spans="1:19" s="88" customFormat="1" ht="16.75" customHeight="1">
+      <c r="A17" s="83"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="84" t="s">
+        <v>766</v>
+      </c>
+      <c r="G17" s="83" t="s">
+        <v>787</v>
+      </c>
+      <c r="H17" s="85" t="s">
+        <v>788</v>
+      </c>
+      <c r="I17" s="85"/>
+      <c r="J17" s="85">
+        <v>1</v>
+      </c>
+      <c r="K17" s="86" t="s">
+        <v>750</v>
+      </c>
+      <c r="L17" s="85"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="85" t="s">
+        <v>789</v>
+      </c>
+      <c r="O17" s="85"/>
+      <c r="P17" s="85" t="s">
+        <v>790</v>
+      </c>
+      <c r="Q17" s="85"/>
+      <c r="R17" s="83"/>
+    </row>
+    <row r="18" spans="1:19" ht="16.75" customHeight="1">
+      <c r="A18" s="74"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="79" t="s">
+        <v>791</v>
+      </c>
+      <c r="G18" s="74" t="s">
+        <v>792</v>
+      </c>
+      <c r="H18" s="76" t="s">
+        <v>793</v>
+      </c>
+      <c r="I18" s="77"/>
+      <c r="J18" s="77">
+        <v>1</v>
+      </c>
+      <c r="K18" s="81" t="s">
+        <v>750</v>
+      </c>
+      <c r="L18" s="77"/>
+      <c r="M18" s="77"/>
+      <c r="N18" s="77" t="s">
+        <v>794</v>
+      </c>
+      <c r="O18" s="77"/>
+      <c r="P18" s="77" t="s">
+        <v>795</v>
+      </c>
+      <c r="Q18" s="77"/>
+      <c r="R18" s="74"/>
+    </row>
+    <row r="19" spans="1:19" ht="16.75" customHeight="1">
+      <c r="E19" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="79" t="s">
+        <v>796</v>
+      </c>
+      <c r="G19" s="60" t="s">
+        <v>797</v>
+      </c>
+      <c r="H19" s="76" t="s">
+        <v>798</v>
+      </c>
+      <c r="J19" s="77">
+        <v>1</v>
+      </c>
+      <c r="K19" s="89" t="s">
+        <v>799</v>
+      </c>
+      <c r="N19" s="77" t="s">
+        <v>800</v>
+      </c>
+      <c r="P19" s="77" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="16.75" customHeight="1">
+      <c r="E20" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="60" t="s">
+        <v>796</v>
+      </c>
+      <c r="G20" s="60" t="s">
+        <v>802</v>
+      </c>
+      <c r="H20" s="76" t="s">
+        <v>803</v>
+      </c>
+      <c r="J20" s="77">
+        <v>1</v>
+      </c>
+      <c r="K20" s="89" t="s">
+        <v>804</v>
+      </c>
+      <c r="N20" s="77" t="s">
+        <v>805</v>
+      </c>
+      <c r="P20" s="90" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="16.75" customHeight="1">
+      <c r="E21" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="60" t="s">
+        <v>766</v>
+      </c>
+      <c r="G21" s="89" t="s">
+        <v>807</v>
+      </c>
+      <c r="H21" s="76" t="s">
+        <v>808</v>
+      </c>
+      <c r="J21" s="77">
+        <v>1</v>
+      </c>
+      <c r="K21" s="81" t="s">
+        <v>750</v>
+      </c>
+      <c r="N21" s="77" t="s">
+        <v>809</v>
+      </c>
+      <c r="P21" s="90" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="16.75" customHeight="1">
+      <c r="C22" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="79" t="s">
+        <v>741</v>
+      </c>
+      <c r="G22" s="60" t="s">
+        <v>811</v>
+      </c>
+      <c r="H22" s="76" t="s">
+        <v>812</v>
+      </c>
+      <c r="J22" s="77">
+        <v>1</v>
+      </c>
+      <c r="K22" s="60" t="s">
+        <v>744</v>
+      </c>
+      <c r="N22" s="77" t="s">
+        <v>813</v>
+      </c>
+      <c r="P22" s="90" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="16.25" customHeight="1"/>
+    <row r="24" spans="1:19" ht="16.75" customHeight="1">
+      <c r="F24" s="60" t="s">
+        <v>741</v>
+      </c>
+      <c r="G24" s="60" t="s">
+        <v>815</v>
+      </c>
+      <c r="H24" s="91" t="s">
+        <v>816</v>
+      </c>
+      <c r="J24" s="77">
+        <v>1</v>
+      </c>
+      <c r="K24" s="81" t="s">
+        <v>750</v>
+      </c>
+      <c r="N24" s="60" t="s">
+        <v>817</v>
+      </c>
+      <c r="P24" s="60" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="16.75" customHeight="1">
+      <c r="F25" s="60" t="s">
+        <v>819</v>
+      </c>
+      <c r="G25" s="60" t="s">
+        <v>820</v>
+      </c>
+      <c r="H25" s="91" t="s">
+        <v>821</v>
+      </c>
+      <c r="J25" s="77">
+        <v>1</v>
+      </c>
+      <c r="K25" s="81" t="s">
+        <v>750</v>
+      </c>
+      <c r="N25" s="60" t="s">
+        <v>822</v>
+      </c>
+      <c r="P25" s="92" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="16.75" customHeight="1">
+      <c r="E26" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="60" t="s">
+        <v>741</v>
+      </c>
+      <c r="G26" s="60" t="s">
+        <v>824</v>
+      </c>
+      <c r="H26" s="91" t="s">
+        <v>825</v>
+      </c>
+      <c r="J26" s="77">
+        <v>1</v>
+      </c>
+      <c r="K26" s="81" t="s">
+        <v>750</v>
+      </c>
+      <c r="N26" s="60" t="s">
+        <v>826</v>
+      </c>
+      <c r="S26" s="60" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="16.75" customHeight="1">
+      <c r="F27" s="60" t="s">
+        <v>777</v>
+      </c>
+      <c r="G27" s="89" t="s">
+        <v>828</v>
+      </c>
+      <c r="H27" s="91" t="s">
+        <v>829</v>
+      </c>
+      <c r="J27" s="77">
+        <v>1</v>
+      </c>
+      <c r="K27" s="81" t="s">
+        <v>750</v>
+      </c>
+      <c r="N27" s="60" t="s">
+        <v>830</v>
+      </c>
+      <c r="P27" s="60" t="s">
+        <v>831</v>
+      </c>
+      <c r="S27" s="93"/>
+    </row>
+    <row r="28" spans="1:19" ht="16.75" customHeight="1">
+      <c r="E28" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="60" t="s">
+        <v>832</v>
+      </c>
+      <c r="G28" s="60" t="s">
+        <v>833</v>
+      </c>
+      <c r="H28" s="91" t="s">
+        <v>834</v>
+      </c>
+      <c r="J28" s="60" t="s">
+        <v>769</v>
+      </c>
+      <c r="K28" s="89" t="s">
+        <v>835</v>
+      </c>
+      <c r="N28" s="60" t="s">
+        <v>836</v>
+      </c>
+      <c r="P28" s="60" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="16.75" customHeight="1">
+      <c r="F29" s="93" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" s="94" customFormat="1" ht="16.75" customHeight="1">
+      <c r="F30" s="94" t="s">
+        <v>839</v>
+      </c>
+      <c r="H30" s="91" t="s">
+        <v>998</v>
+      </c>
+      <c r="J30" s="94" t="s">
+        <v>840</v>
+      </c>
+      <c r="K30" s="95" t="s">
+        <v>804</v>
+      </c>
+      <c r="N30" s="94" t="s">
+        <v>841</v>
+      </c>
+      <c r="P30" s="96" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="16.75" customHeight="1">
+      <c r="F31" s="60" t="s">
+        <v>777</v>
+      </c>
+      <c r="H31" s="91" t="s">
+        <v>999</v>
+      </c>
+      <c r="J31" s="60">
+        <v>1</v>
+      </c>
+      <c r="K31" s="81" t="s">
+        <v>750</v>
+      </c>
+      <c r="N31" s="60" t="s">
+        <v>843</v>
+      </c>
+      <c r="P31" s="97" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="16.75" customHeight="1">
+      <c r="E32" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="60" t="s">
+        <v>844</v>
+      </c>
+      <c r="H32" s="91" t="s">
+        <v>845</v>
+      </c>
+      <c r="J32" s="60">
+        <v>1</v>
+      </c>
+      <c r="K32" s="60" t="s">
+        <v>846</v>
+      </c>
+      <c r="N32" s="60" t="s">
+        <v>847</v>
+      </c>
+      <c r="P32" s="98" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F33" s="60" t="s">
+        <v>791</v>
+      </c>
+      <c r="G33" s="63" t="s">
+        <v>849</v>
+      </c>
+      <c r="H33" s="91" t="s">
+        <v>850</v>
+      </c>
+      <c r="J33" s="60">
+        <v>1</v>
+      </c>
+      <c r="K33" s="60" t="s">
+        <v>799</v>
+      </c>
+      <c r="N33" s="60" t="s">
+        <v>851</v>
+      </c>
+      <c r="P33" s="99" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="34" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F34" s="60" t="s">
+        <v>853</v>
+      </c>
+      <c r="H34" s="91" t="s">
+        <v>854</v>
+      </c>
+      <c r="J34" s="60">
+        <v>1</v>
+      </c>
+      <c r="K34" s="60" t="s">
+        <v>763</v>
+      </c>
+      <c r="N34" s="60" t="s">
+        <v>855</v>
+      </c>
+      <c r="P34" s="90" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F35" s="60" t="s">
+        <v>857</v>
+      </c>
+      <c r="G35" s="100"/>
+      <c r="H35" s="91" t="s">
+        <v>858</v>
+      </c>
+      <c r="J35" s="60">
+        <v>1</v>
+      </c>
+      <c r="K35" s="60" t="s">
+        <v>859</v>
+      </c>
+      <c r="N35" s="60" t="s">
+        <v>860</v>
+      </c>
+      <c r="P35" s="60" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16" ht="16.75" customHeight="1">
+      <c r="E36" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="60" t="s">
+        <v>862</v>
+      </c>
+      <c r="G36" s="60" t="s">
+        <v>863</v>
+      </c>
+      <c r="H36" s="101" t="s">
+        <v>864</v>
+      </c>
+      <c r="J36" s="102"/>
+      <c r="N36" s="60" t="s">
+        <v>865</v>
+      </c>
+      <c r="P36" s="60" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="37" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F37" s="60" t="s">
+        <v>857</v>
+      </c>
+      <c r="G37" s="100"/>
+      <c r="H37" s="91" t="s">
+        <v>867</v>
+      </c>
+      <c r="J37" s="60" t="s">
+        <v>769</v>
+      </c>
+      <c r="K37" s="60" t="s">
+        <v>868</v>
+      </c>
+      <c r="N37" s="60" t="s">
+        <v>869</v>
+      </c>
+      <c r="P37" s="103" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="38" spans="3:16" ht="16.75" customHeight="1">
+      <c r="D38" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="60" t="s">
+        <v>741</v>
+      </c>
+      <c r="G38" s="60" t="s">
+        <v>871</v>
+      </c>
+      <c r="H38" s="91" t="s">
+        <v>872</v>
+      </c>
+      <c r="J38" s="60">
+        <v>1</v>
+      </c>
+      <c r="K38" s="60" t="s">
+        <v>799</v>
+      </c>
+      <c r="N38" s="60" t="s">
+        <v>873</v>
+      </c>
+      <c r="P38" s="60" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="39" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F39" s="60" t="s">
+        <v>741</v>
+      </c>
+      <c r="H39" s="91" t="s">
+        <v>875</v>
+      </c>
+      <c r="K39" s="60" t="s">
+        <v>744</v>
+      </c>
+      <c r="N39" s="60" t="s">
+        <v>876</v>
+      </c>
+      <c r="P39" s="104" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="40" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F40" s="60" t="s">
+        <v>741</v>
+      </c>
+      <c r="G40" s="60" t="s">
+        <v>878</v>
+      </c>
+      <c r="H40" s="91" t="s">
+        <v>879</v>
+      </c>
+      <c r="J40" s="98">
+        <v>1</v>
+      </c>
+      <c r="K40" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N40" s="60" t="s">
+        <v>880</v>
+      </c>
+      <c r="P40" s="98" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="41" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F41" s="60" t="s">
+        <v>741</v>
+      </c>
+      <c r="G41" s="60" t="s">
+        <v>882</v>
+      </c>
+      <c r="H41" s="91" t="s">
+        <v>883</v>
+      </c>
+      <c r="J41" s="60">
+        <v>1</v>
+      </c>
+      <c r="K41" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N41" s="60" t="s">
+        <v>884</v>
+      </c>
+      <c r="P41" s="105" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="42" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F42" s="60" t="s">
+        <v>741</v>
+      </c>
+      <c r="G42" s="63" t="s">
+        <v>886</v>
+      </c>
+      <c r="H42" s="91" t="s">
+        <v>887</v>
+      </c>
+      <c r="J42" s="60">
+        <v>1</v>
+      </c>
+      <c r="K42" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N42" s="60" t="s">
+        <v>888</v>
+      </c>
+      <c r="P42" s="98" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="44" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F44" s="93" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="45" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F45" s="60" t="s">
+        <v>891</v>
+      </c>
+      <c r="G45" s="60" t="s">
+        <v>892</v>
+      </c>
+      <c r="H45" s="91" t="s">
+        <v>893</v>
+      </c>
+      <c r="J45" s="60">
+        <v>1</v>
+      </c>
+      <c r="K45" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N45" s="60" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="46" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F46" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="60" t="s">
+        <v>895</v>
+      </c>
+      <c r="H46" s="91" t="s">
+        <v>896</v>
+      </c>
+      <c r="J46" s="60">
+        <v>1</v>
+      </c>
+      <c r="K46" s="60" t="s">
+        <v>738</v>
+      </c>
+      <c r="N46" s="60" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="47" spans="3:16" ht="16.75" customHeight="1">
+      <c r="F47" s="60" t="s">
+        <v>891</v>
+      </c>
+      <c r="G47" s="60" t="s">
+        <v>898</v>
+      </c>
+      <c r="H47" s="91" t="s">
+        <v>899</v>
+      </c>
+      <c r="J47" s="60">
+        <v>1</v>
+      </c>
+      <c r="K47" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N47" s="60" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="48" spans="3:16" ht="16.75" customHeight="1">
+      <c r="C48" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="60" t="s">
+        <v>901</v>
+      </c>
+      <c r="H48" s="91" t="s">
+        <v>902</v>
+      </c>
+      <c r="J48" s="60">
+        <v>1</v>
+      </c>
+      <c r="K48" s="60" t="s">
+        <v>903</v>
+      </c>
+      <c r="N48" s="60" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" ht="16.75" customHeight="1">
+      <c r="B49" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="60" t="s">
+        <v>905</v>
+      </c>
+      <c r="G49" s="60" t="s">
+        <v>906</v>
+      </c>
+      <c r="H49" s="91" t="s">
+        <v>907</v>
+      </c>
+      <c r="J49" s="60">
+        <v>1</v>
+      </c>
+      <c r="K49" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N49" s="60" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" ht="16.75" customHeight="1">
+      <c r="F50" s="60" t="s">
+        <v>909</v>
+      </c>
+      <c r="G50" s="60" t="s">
+        <v>910</v>
+      </c>
+      <c r="H50" s="91" t="s">
+        <v>911</v>
+      </c>
+      <c r="J50" s="60">
+        <v>1</v>
+      </c>
+      <c r="K50" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N50" s="60" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" ht="16.75" customHeight="1">
+      <c r="F51" s="60" t="s">
+        <v>913</v>
+      </c>
+      <c r="G51" s="60" t="s">
+        <v>914</v>
+      </c>
+      <c r="H51" s="91" t="s">
+        <v>915</v>
+      </c>
+      <c r="J51" s="60">
+        <v>1</v>
+      </c>
+      <c r="K51" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N51" s="60" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" ht="16.75" customHeight="1">
+      <c r="F52" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="60" t="s">
+        <v>917</v>
+      </c>
+      <c r="H52" s="91" t="s">
+        <v>918</v>
+      </c>
+      <c r="J52" s="60">
+        <v>1</v>
+      </c>
+      <c r="N52" s="60" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" ht="16.75" customHeight="1">
+      <c r="F53" s="60" t="s">
+        <v>891</v>
+      </c>
+      <c r="G53" s="60" t="s">
+        <v>920</v>
+      </c>
+      <c r="H53" s="91" t="s">
+        <v>921</v>
+      </c>
+      <c r="J53" s="60">
+        <v>1</v>
+      </c>
+      <c r="K53" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N53" s="60" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" ht="16.75" customHeight="1">
+      <c r="C54" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="60" t="s">
+        <v>923</v>
+      </c>
+      <c r="H54" s="91" t="s">
+        <v>924</v>
+      </c>
+      <c r="J54" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" ht="16.75" customHeight="1">
+      <c r="C55" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" s="60" t="s">
+        <v>925</v>
+      </c>
+      <c r="G55" s="106"/>
+      <c r="H55" s="91" t="s">
+        <v>926</v>
+      </c>
+      <c r="J55" s="60">
+        <v>1</v>
+      </c>
+      <c r="K55" s="60" t="s">
+        <v>927</v>
+      </c>
+      <c r="N55" s="60" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" ht="16.75" customHeight="1">
+      <c r="E56" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" s="60" t="s">
+        <v>905</v>
+      </c>
+      <c r="G56" s="60" t="s">
+        <v>929</v>
+      </c>
+      <c r="H56" s="91" t="s">
+        <v>930</v>
+      </c>
+      <c r="J56" s="60" t="s">
+        <v>931</v>
+      </c>
+      <c r="K56" s="60" t="s">
+        <v>932</v>
+      </c>
+      <c r="N56" s="60" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" ht="16.75" customHeight="1">
+      <c r="E57" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F57" s="60" t="s">
+        <v>934</v>
+      </c>
+      <c r="G57" s="60" t="s">
+        <v>935</v>
+      </c>
+      <c r="H57" s="91" t="s">
+        <v>936</v>
+      </c>
+      <c r="J57" s="60">
+        <v>1</v>
+      </c>
+      <c r="K57" s="60" t="s">
+        <v>937</v>
+      </c>
+      <c r="N57" s="60" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" s="107" customFormat="1" ht="16.75" customHeight="1">
+      <c r="C58" s="107" t="s">
+        <v>5</v>
+      </c>
+      <c r="F58" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" s="107" t="s">
+        <v>939</v>
+      </c>
+      <c r="H58" s="107" t="s">
+        <v>940</v>
+      </c>
+      <c r="J58" s="107">
+        <v>1</v>
+      </c>
+      <c r="K58" s="107" t="s">
+        <v>750</v>
+      </c>
+      <c r="N58" s="107" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" ht="16.75" customHeight="1">
+      <c r="F59" s="60" t="s">
+        <v>891</v>
+      </c>
+      <c r="G59" s="60" t="s">
+        <v>942</v>
+      </c>
+      <c r="H59" s="91" t="s">
+        <v>943</v>
+      </c>
+      <c r="J59" s="60">
+        <v>1</v>
+      </c>
+      <c r="K59" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N59" s="60" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" ht="16.75" customHeight="1">
+      <c r="B60" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="60" t="s">
+        <v>905</v>
+      </c>
+      <c r="G60" s="89" t="s">
+        <v>945</v>
+      </c>
+      <c r="H60" s="101" t="s">
+        <v>946</v>
+      </c>
+      <c r="K60" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N60" s="60" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="61" spans="2:14" ht="16.75" customHeight="1">
+      <c r="D61" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" s="89" t="s">
+        <v>948</v>
+      </c>
+      <c r="H61" s="91" t="s">
+        <v>949</v>
+      </c>
+      <c r="J61" s="60">
+        <v>1</v>
+      </c>
+      <c r="K61" s="60" t="s">
+        <v>927</v>
+      </c>
+      <c r="N61" s="60" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" ht="16.75" customHeight="1">
+      <c r="F62" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G62" s="60" t="s">
+        <v>951</v>
+      </c>
+      <c r="H62" s="91" t="s">
+        <v>952</v>
+      </c>
+      <c r="J62" s="60">
+        <v>1</v>
+      </c>
+      <c r="N62" s="60" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14" ht="16.75" customHeight="1">
+      <c r="F63" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G63" s="60" t="s">
+        <v>954</v>
+      </c>
+      <c r="H63" s="91" t="s">
+        <v>955</v>
+      </c>
+      <c r="J63" s="60">
+        <v>1</v>
+      </c>
+      <c r="N63" s="60" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" ht="16.75" customHeight="1">
+      <c r="E64" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" s="60" t="s">
+        <v>957</v>
+      </c>
+      <c r="G64" s="60" t="s">
+        <v>958</v>
+      </c>
+      <c r="H64" s="91" t="s">
+        <v>959</v>
+      </c>
+      <c r="J64" s="60">
+        <v>1</v>
+      </c>
+      <c r="N64" s="60" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" ht="16.75" customHeight="1">
+      <c r="C65" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G65" s="60" t="s">
+        <v>961</v>
+      </c>
+      <c r="H65" s="91" t="s">
+        <v>962</v>
+      </c>
+      <c r="J65" s="60">
+        <v>1</v>
+      </c>
+      <c r="K65" s="60" t="s">
+        <v>750</v>
+      </c>
+      <c r="N65" s="60" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" ht="16.75" customHeight="1">
+      <c r="F66" s="60" t="s">
+        <v>964</v>
+      </c>
+      <c r="G66" s="106"/>
+      <c r="H66" s="91" t="s">
+        <v>965</v>
+      </c>
+      <c r="J66" s="60">
+        <v>1</v>
+      </c>
+      <c r="K66" s="60" t="s">
+        <v>744</v>
+      </c>
+      <c r="N66" s="60" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" ht="16.75" customHeight="1">
+      <c r="B67" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" s="60" t="s">
+        <v>967</v>
+      </c>
+      <c r="G67" s="60" t="s">
+        <v>968</v>
+      </c>
+      <c r="H67" s="101" t="s">
+        <v>969</v>
+      </c>
+      <c r="N67" s="60" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" ht="16.75" customHeight="1">
+      <c r="H68" s="91" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" ht="16.75" customHeight="1">
+      <c r="F69" s="60" t="s">
+        <v>972</v>
+      </c>
+      <c r="G69" s="60" t="s">
+        <v>973</v>
+      </c>
+      <c r="H69" s="108" t="s">
+        <v>974</v>
+      </c>
+      <c r="K69" s="60" t="s">
+        <v>975</v>
+      </c>
+      <c r="N69" s="60" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" ht="16.75" customHeight="1">
+      <c r="F70" s="60" t="s">
+        <v>972</v>
+      </c>
+      <c r="G70" s="60" t="s">
+        <v>977</v>
+      </c>
+      <c r="H70" s="108" t="s">
+        <v>978</v>
+      </c>
+      <c r="K70" s="60" t="s">
+        <v>763</v>
+      </c>
+      <c r="N70" s="60" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" ht="16.75" customHeight="1">
+      <c r="F72" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="H72" s="91" t="s">
+        <v>980</v>
+      </c>
+      <c r="K72" s="60" t="s">
+        <v>981</v>
+      </c>
+      <c r="N72" s="60" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" ht="16.75" customHeight="1">
+      <c r="F73" s="60" t="s">
+        <v>905</v>
+      </c>
+      <c r="H73" s="91" t="s">
+        <v>983</v>
+      </c>
+      <c r="K73" s="60" t="s">
+        <v>744</v>
+      </c>
+      <c r="N73" s="60" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A74" s="61"/>
+      <c r="B74" s="61"/>
+      <c r="C74" s="61"/>
+      <c r="D74" s="61"/>
+      <c r="E74" s="61"/>
+      <c r="F74" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="G74" s="63" t="s">
+        <v>985</v>
+      </c>
+      <c r="H74" s="64" t="s">
+        <v>986</v>
+      </c>
+      <c r="I74" s="65"/>
+      <c r="J74" s="65"/>
+      <c r="K74" s="65" t="s">
+        <v>750</v>
+      </c>
+      <c r="L74" s="65"/>
+      <c r="M74" s="66"/>
+      <c r="N74" s="109" t="s">
+        <v>987</v>
+      </c>
+      <c r="O74" s="65"/>
+      <c r="P74" s="65"/>
+      <c r="Q74" s="65"/>
+      <c r="R74" s="61"/>
+    </row>
+    <row r="75" spans="1:18" ht="16.75" customHeight="1">
+      <c r="A75" s="61"/>
+      <c r="B75" s="61"/>
+      <c r="C75" s="61"/>
+      <c r="D75" s="61"/>
+      <c r="E75" s="61"/>
+      <c r="F75" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="G75" s="63" t="s">
+        <v>988</v>
+      </c>
+      <c r="H75" s="64" t="s">
+        <v>989</v>
+      </c>
+      <c r="I75" s="65"/>
+      <c r="J75" s="65"/>
+      <c r="K75" s="65"/>
+      <c r="L75" s="65"/>
+      <c r="M75" s="66"/>
+      <c r="N75" s="65"/>
+      <c r="O75" s="65"/>
+      <c r="P75" s="65"/>
+      <c r="Q75" s="65"/>
+      <c r="R75" s="61"/>
+    </row>
+    <row r="76" spans="1:18" ht="16.75" customHeight="1">
+      <c r="F76" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="G76" s="60" t="s">
+        <v>990</v>
+      </c>
+      <c r="H76" s="91" t="s">
+        <v>991</v>
+      </c>
+      <c r="K76" s="65" t="s">
+        <v>750</v>
+      </c>
+      <c r="N76" s="60" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" ht="16.75" customHeight="1">
+      <c r="F77" s="60" t="s">
+        <v>891</v>
+      </c>
+      <c r="G77" s="60" t="s">
+        <v>993</v>
+      </c>
+      <c r="H77" s="91" t="s">
+        <v>994</v>
+      </c>
+      <c r="K77" s="65" t="s">
+        <v>750</v>
+      </c>
+      <c r="N77" s="60" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" ht="16.75" customHeight="1">
+      <c r="F79" s="60" t="s">
+        <v>996</v>
+      </c>
+      <c r="H79" s="91" t="s">
+        <v>930</v>
+      </c>
+      <c r="K79" s="65" t="s">
+        <v>932</v>
+      </c>
+      <c r="N79" s="60" t="s">
+        <v>997</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G74" r:id="rId1"/>
+    <hyperlink ref="G75" r:id="rId2"/>
+    <hyperlink ref="G33" r:id="rId3"/>
+    <hyperlink ref="G42" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G4" r:id="rId6"/>
+    <hyperlink ref="G8" r:id="rId7"/>
+    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G10" r:id="rId9"/>
+    <hyperlink ref="K11" r:id="rId10"/>
+    <hyperlink ref="K8" r:id="rId11"/>
+    <hyperlink ref="K9" r:id="rId12"/>
+    <hyperlink ref="K12" r:id="rId13"/>
+    <hyperlink ref="K14" r:id="rId14"/>
+    <hyperlink ref="K13" r:id="rId15"/>
+    <hyperlink ref="G14" r:id="rId16"/>
+    <hyperlink ref="K17" r:id="rId17"/>
+    <hyperlink ref="K18" r:id="rId18"/>
+    <hyperlink ref="K20" r:id="rId19"/>
+    <hyperlink ref="K21" r:id="rId20"/>
+    <hyperlink ref="K24" r:id="rId21"/>
+    <hyperlink ref="K25" r:id="rId22"/>
+    <hyperlink ref="K28" r:id="rId23"/>
+    <hyperlink ref="G27" r:id="rId24"/>
+    <hyperlink ref="K26" r:id="rId25"/>
+    <hyperlink ref="K27" r:id="rId26"/>
+    <hyperlink ref="K30" r:id="rId27"/>
+    <hyperlink ref="K31" r:id="rId28"/>
+    <hyperlink ref="G61" r:id="rId29"/>
+    <hyperlink ref="G60" r:id="rId30"/>
+    <hyperlink ref="G21" r:id="rId31"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D31"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
@@ -6068,7 +9122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C17"/>
   <sheetViews>
@@ -6212,7 +9266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C6"/>
   <sheetViews>
@@ -6268,7 +9322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C6"/>
   <sheetViews>
@@ -6318,7 +9372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C10"/>
   <sheetViews>
@@ -6403,7 +9457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D7"/>
   <sheetViews>
@@ -6468,7 +9522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>